<commit_message>
Added counter command and fixed some odd cases for cooldowns
Co-authored-by: Thundeee <Thundeee@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/constants/cooldowns.xlsx
+++ b/constants/cooldowns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Bureaublad\League Bot (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Bureaublad\League Bot (2)\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB63EB89-BB7A-4E92-B309-5C06F89F2C79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7AAF639-0BDD-4CEC-B21B-5922D0AC2222}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B29662F5-47C4-4CA1-BD97-0B128CDABFDA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="588">
   <si>
     <t>Champion</t>
   </si>
@@ -941,12 +941,6 @@
     <t>Quinn</t>
   </si>
   <si>
-    <t>8-2.93s</t>
-  </si>
-  <si>
-    <t>Passive cooldown is based on critical strike chance.</t>
-  </si>
-  <si>
     <t>R has a cast time of 2s.</t>
   </si>
   <si>
@@ -1752,9 +1746,6 @@
   </si>
   <si>
     <t>Level 1 - 18 **2.5s**</t>
-  </si>
-  <si>
-    <t>Level 1 - 18 **34s**</t>
   </si>
   <si>
     <t>Level 1 - 18 **30s**</t>
@@ -1801,6 +1792,15 @@
   </si>
   <si>
     <t>Level 1 **13s**%n Level 5 **12s**%n Level 9 **11s**%n Level 13 **10s**%n Level 18 **9s**%</t>
+  </si>
+  <si>
+    <t>34s</t>
+  </si>
+  <si>
+    <t>0% Crit Chance **8s**%n100% Crit Chance **2.93s**%n (Scales every 10% Crit Chance)</t>
+  </si>
+  <si>
+    <t>Base CD on basic abilities is reduced with **R** ranks : **10/25/40%**</t>
   </si>
 </sst>
 </file>
@@ -2439,7 +2439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2696,9 +2696,6 @@
     <xf numFmtId="0" fontId="10" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2713,9 +2710,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2735,6 +2729,18 @@
     <xf numFmtId="0" fontId="5" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2753,59 +2759,59 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2918,23 +2924,8 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3253,15 +3244,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6840B42-881F-4D54-A75C-44FD07512C15}">
   <dimension ref="A1:W871"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A772" workbookViewId="0">
-      <selection activeCell="Z767" sqref="Z767"/>
+    <sheetView tabSelected="1" topLeftCell="A760" workbookViewId="0">
+      <selection activeCell="A760" sqref="A1:W871"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3327,7 +3318,7 @@
         <v>20</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.35">
@@ -3391,11 +3382,11 @@
       <c r="T2" s="16">
         <v>100</v>
       </c>
-      <c r="U2" s="96">
+      <c r="U2" s="94">
         <v>80</v>
       </c>
-      <c r="V2" s="97" t="s">
-        <v>551</v>
+      <c r="V2" s="95" t="s">
+        <v>549</v>
       </c>
       <c r="W2" s="18" t="s">
         <v>23</v>
@@ -3423,7 +3414,7 @@
       <c r="S3" s="25"/>
       <c r="T3" s="25"/>
       <c r="U3" s="25"/>
-      <c r="V3" s="94"/>
+      <c r="V3" s="92"/>
       <c r="W3" s="18" t="s">
         <v>24</v>
       </c>
@@ -3450,7 +3441,7 @@
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="25"/>
-      <c r="V4" s="94"/>
+      <c r="V4" s="92"/>
       <c r="W4" s="18" t="s">
         <v>25</v>
       </c>
@@ -3506,7 +3497,7 @@
       <c r="U6" s="33"/>
       <c r="V6" s="34"/>
       <c r="W6" s="52" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3572,7 +3563,7 @@
         <v>80</v>
       </c>
       <c r="V7" s="17" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="W7" s="18" t="s">
         <v>28</v>
@@ -3914,7 +3905,7 @@
         <v>80</v>
       </c>
       <c r="V17" s="17" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="W17" s="18" t="s">
         <v>37</v>
@@ -4248,7 +4239,7 @@
         <v>2</v>
       </c>
       <c r="V27" s="17" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="W27" s="18" t="s">
         <v>42</v>
@@ -4546,20 +4537,20 @@
       <c r="H37" s="42">
         <v>9</v>
       </c>
-      <c r="I37" s="132" t="s">
+      <c r="I37" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="J37" s="133"/>
-      <c r="K37" s="134" t="s">
+      <c r="J37" s="135"/>
+      <c r="K37" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="L37" s="135"/>
-      <c r="M37" s="135"/>
-      <c r="N37" s="135"/>
-      <c r="O37" s="135"/>
-      <c r="P37" s="135"/>
-      <c r="Q37" s="135"/>
-      <c r="R37" s="136"/>
+      <c r="L37" s="137"/>
+      <c r="M37" s="137"/>
+      <c r="N37" s="137"/>
+      <c r="O37" s="137"/>
+      <c r="P37" s="137"/>
+      <c r="Q37" s="137"/>
+      <c r="R37" s="138"/>
       <c r="S37" s="16">
         <v>120</v>
       </c>
@@ -4597,18 +4588,18 @@
       <c r="H38" s="42">
         <v>8.25</v>
       </c>
-      <c r="I38" s="143" t="s">
+      <c r="I38" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="J38" s="144"/>
-      <c r="K38" s="137"/>
-      <c r="L38" s="138"/>
-      <c r="M38" s="138"/>
-      <c r="N38" s="138"/>
-      <c r="O38" s="138"/>
-      <c r="P38" s="138"/>
-      <c r="Q38" s="138"/>
-      <c r="R38" s="139"/>
+      <c r="J38" s="146"/>
+      <c r="K38" s="139"/>
+      <c r="L38" s="140"/>
+      <c r="M38" s="140"/>
+      <c r="N38" s="140"/>
+      <c r="O38" s="140"/>
+      <c r="P38" s="140"/>
+      <c r="Q38" s="140"/>
+      <c r="R38" s="141"/>
       <c r="S38" s="25">
         <v>120</v>
       </c>
@@ -4646,18 +4637,18 @@
       <c r="H39" s="42">
         <v>7.5</v>
       </c>
-      <c r="I39" s="145" t="s">
+      <c r="I39" s="147" t="s">
         <v>55</v>
       </c>
-      <c r="J39" s="146"/>
-      <c r="K39" s="137"/>
-      <c r="L39" s="138"/>
-      <c r="M39" s="138"/>
-      <c r="N39" s="138"/>
-      <c r="O39" s="138"/>
-      <c r="P39" s="138"/>
-      <c r="Q39" s="138"/>
-      <c r="R39" s="139"/>
+      <c r="J39" s="148"/>
+      <c r="K39" s="139"/>
+      <c r="L39" s="140"/>
+      <c r="M39" s="140"/>
+      <c r="N39" s="140"/>
+      <c r="O39" s="140"/>
+      <c r="P39" s="140"/>
+      <c r="Q39" s="140"/>
+      <c r="R39" s="141"/>
       <c r="S39" s="25">
         <v>120</v>
       </c>
@@ -4693,18 +4684,18 @@
       <c r="H40" s="42">
         <v>6.75</v>
       </c>
-      <c r="I40" s="147" t="s">
+      <c r="I40" s="149" t="s">
         <v>57</v>
       </c>
-      <c r="J40" s="148"/>
-      <c r="K40" s="137"/>
-      <c r="L40" s="138"/>
-      <c r="M40" s="138"/>
-      <c r="N40" s="138"/>
-      <c r="O40" s="138"/>
-      <c r="P40" s="138"/>
-      <c r="Q40" s="138"/>
-      <c r="R40" s="139"/>
+      <c r="J40" s="150"/>
+      <c r="K40" s="139"/>
+      <c r="L40" s="140"/>
+      <c r="M40" s="140"/>
+      <c r="N40" s="140"/>
+      <c r="O40" s="140"/>
+      <c r="P40" s="140"/>
+      <c r="Q40" s="140"/>
+      <c r="R40" s="141"/>
       <c r="S40" s="25">
         <v>120</v>
       </c>
@@ -4742,18 +4733,18 @@
       <c r="H41" s="50">
         <v>6</v>
       </c>
-      <c r="I41" s="149" t="s">
+      <c r="I41" s="151" t="s">
         <v>60</v>
       </c>
-      <c r="J41" s="150"/>
-      <c r="K41" s="140"/>
-      <c r="L41" s="141"/>
-      <c r="M41" s="141"/>
-      <c r="N41" s="141"/>
-      <c r="O41" s="141"/>
-      <c r="P41" s="141"/>
-      <c r="Q41" s="141"/>
-      <c r="R41" s="142"/>
+      <c r="J41" s="152"/>
+      <c r="K41" s="142"/>
+      <c r="L41" s="143"/>
+      <c r="M41" s="143"/>
+      <c r="N41" s="143"/>
+      <c r="O41" s="143"/>
+      <c r="P41" s="143"/>
+      <c r="Q41" s="143"/>
+      <c r="R41" s="144"/>
       <c r="S41" s="51">
         <v>120</v>
       </c>
@@ -5151,7 +5142,7 @@
         <v>90</v>
       </c>
       <c r="V52" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="W52" s="18" t="s">
         <v>66</v>
@@ -5426,7 +5417,7 @@
       <c r="V61" s="34"/>
       <c r="W61" s="35"/>
     </row>
-    <row r="62" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="11" t="s">
         <v>72</v>
@@ -5488,8 +5479,8 @@
       <c r="U62" s="16">
         <v>20</v>
       </c>
-      <c r="V62" s="164" t="s">
-        <v>565</v>
+      <c r="V62" s="17" t="s">
+        <v>563</v>
       </c>
       <c r="W62" s="18"/>
     </row>
@@ -5825,9 +5816,9 @@
         <v>80</v>
       </c>
       <c r="V72" s="67" t="s">
-        <v>553</v>
-      </c>
-      <c r="W72" s="160" t="s">
+        <v>551</v>
+      </c>
+      <c r="W72" s="97" t="s">
         <v>77</v>
       </c>
     </row>
@@ -5853,8 +5844,8 @@
       <c r="S73" s="25"/>
       <c r="T73" s="25"/>
       <c r="U73" s="25"/>
-      <c r="V73" s="94"/>
-      <c r="W73" s="161">
+      <c r="V73" s="92"/>
+      <c r="W73" s="98">
         <v>41456</v>
       </c>
     </row>
@@ -5880,9 +5871,9 @@
       <c r="S74" s="25"/>
       <c r="T74" s="25"/>
       <c r="U74" s="25"/>
-      <c r="V74" s="94"/>
-      <c r="W74" s="160" t="s">
-        <v>544</v>
+      <c r="V74" s="92"/>
+      <c r="W74" s="97" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="75" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -5907,8 +5898,8 @@
       <c r="S75" s="25"/>
       <c r="T75" s="25"/>
       <c r="U75" s="25"/>
-      <c r="V75" s="94"/>
-      <c r="W75" s="161">
+      <c r="V75" s="92"/>
+      <c r="W75" s="98">
         <v>38906</v>
       </c>
     </row>
@@ -5935,8 +5926,8 @@
       <c r="T76" s="33"/>
       <c r="U76" s="33"/>
       <c r="V76" s="79"/>
-      <c r="W76" s="162" t="s">
-        <v>545</v>
+      <c r="W76" s="99" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="77" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6171,9 +6162,9 @@
         <v>90</v>
       </c>
       <c r="V82" s="67" t="s">
-        <v>554</v>
-      </c>
-      <c r="W82" s="163" t="s">
+        <v>552</v>
+      </c>
+      <c r="W82" s="100" t="s">
         <v>77</v>
       </c>
     </row>
@@ -6199,8 +6190,8 @@
       <c r="S83" s="25"/>
       <c r="T83" s="25"/>
       <c r="U83" s="25"/>
-      <c r="V83" s="94"/>
-      <c r="W83" s="161">
+      <c r="V83" s="92"/>
+      <c r="W83" s="98">
         <v>41456</v>
       </c>
     </row>
@@ -6226,9 +6217,9 @@
       <c r="S84" s="25"/>
       <c r="T84" s="25"/>
       <c r="U84" s="25"/>
-      <c r="V84" s="94"/>
-      <c r="W84" s="160" t="s">
-        <v>544</v>
+      <c r="V84" s="92"/>
+      <c r="W84" s="97" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="85" spans="1:23" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -6253,9 +6244,9 @@
       <c r="S85" s="25"/>
       <c r="T85" s="25"/>
       <c r="U85" s="25"/>
-      <c r="V85" s="94"/>
-      <c r="W85" s="160" t="s">
-        <v>546</v>
+      <c r="V85" s="92"/>
+      <c r="W85" s="97" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="86" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6676,7 +6667,7 @@
         <v>10</v>
       </c>
       <c r="V97" s="17" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="W97" s="18" t="s">
         <v>85</v>
@@ -7525,7 +7516,7 @@
         <v>50</v>
       </c>
       <c r="V122" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="W122" s="18" t="s">
         <v>106</v>
@@ -7634,7 +7625,7 @@
     <row r="127" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="19"/>
       <c r="B127" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C127" s="12">
         <v>0</v>
@@ -7799,7 +7790,7 @@
     <row r="132" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="19"/>
       <c r="B132" s="11" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C132" s="12">
         <v>0</v>
@@ -8024,7 +8015,7 @@
         <v>80</v>
       </c>
       <c r="V137" s="17" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="W137" s="18" t="s">
         <v>108</v>
@@ -8877,7 +8868,7 @@
         <v>160</v>
       </c>
       <c r="V162" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="W162" s="55" t="s">
         <v>128</v>
@@ -9048,7 +9039,7 @@
         <v>140</v>
       </c>
       <c r="V167" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="W167" s="18" t="s">
         <v>131</v>
@@ -9158,7 +9149,7 @@
       <c r="V171" s="34"/>
       <c r="W171" s="35"/>
     </row>
-    <row r="172" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="19"/>
       <c r="B172" s="11" t="s">
         <v>134</v>
@@ -9220,8 +9211,8 @@
       <c r="U172" s="16">
         <v>80</v>
       </c>
-      <c r="V172" s="164" t="s">
-        <v>568</v>
+      <c r="V172" s="17" t="s">
+        <v>566</v>
       </c>
       <c r="W172" s="18"/>
     </row>
@@ -9388,7 +9379,7 @@
         <v>30</v>
       </c>
       <c r="V177" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="W177" s="18" t="s">
         <v>136</v>
@@ -9565,7 +9556,7 @@
         <v>80</v>
       </c>
       <c r="V182" s="17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="W182" s="18" t="s">
         <v>142</v>
@@ -10249,7 +10240,7 @@
         <v>70</v>
       </c>
       <c r="V202" s="17" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W202" s="52" t="s">
         <v>157</v>
@@ -10931,7 +10922,7 @@
         <v>90</v>
       </c>
       <c r="V222" s="17" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="W222" s="18" t="s">
         <v>172</v>
@@ -11207,7 +11198,7 @@
     <row r="232" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="19"/>
       <c r="B232" s="11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C232" s="12">
         <v>0</v>
@@ -11267,7 +11258,7 @@
         <v>10</v>
       </c>
       <c r="V232" s="16" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="W232" s="18" t="s">
         <v>176</v>
@@ -11378,7 +11369,7 @@
     <row r="237" spans="1:23" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="19"/>
       <c r="B237" s="20" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C237" s="12">
         <v>0</v>
@@ -11437,8 +11428,8 @@
       <c r="U237" s="15">
         <v>16</v>
       </c>
-      <c r="V237" s="165" t="s">
-        <v>570</v>
+      <c r="V237" s="25" t="s">
+        <v>568</v>
       </c>
       <c r="W237" s="18"/>
     </row>
@@ -11605,7 +11596,7 @@
         <v>90</v>
       </c>
       <c r="V242" s="17" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="W242" s="55" t="s">
         <v>179</v>
@@ -12281,7 +12272,7 @@
         <v>36</v>
       </c>
       <c r="V262" s="16" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
       <c r="W262" s="18" t="s">
         <v>190</v>
@@ -12311,7 +12302,7 @@
       <c r="U263" s="25"/>
       <c r="V263" s="25"/>
       <c r="W263" s="18" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="264" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -13068,7 +13059,7 @@
     <row r="287" spans="1:23" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="19"/>
       <c r="B287" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C287" s="12">
         <v>0</v>
@@ -13217,7 +13208,7 @@
       <c r="T290" s="25"/>
       <c r="U290" s="25"/>
       <c r="V290" s="26"/>
-      <c r="W290" s="98"/>
+      <c r="W290" s="96"/>
     </row>
     <row r="291" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="27"/>
@@ -13247,7 +13238,7 @@
     <row r="292" spans="1:23" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="19"/>
       <c r="B292" s="11" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C292" s="12">
         <v>0</v>
@@ -13307,7 +13298,7 @@
         <v>80</v>
       </c>
       <c r="V292" s="17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="W292" s="43" t="s">
         <v>203</v>
@@ -13388,7 +13379,7 @@
       <c r="T295" s="25"/>
       <c r="U295" s="25"/>
       <c r="V295" s="26"/>
-      <c r="W295" s="98"/>
+      <c r="W295" s="96"/>
     </row>
     <row r="296" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="27"/>
@@ -13647,7 +13638,7 @@
         <v>120</v>
       </c>
       <c r="V302" s="17" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="W302" s="18" t="s">
         <v>212</v>
@@ -13824,7 +13815,7 @@
         <v>120</v>
       </c>
       <c r="V307" s="17" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="W307" s="18" t="s">
         <v>218</v>
@@ -14168,7 +14159,7 @@
         <v>30</v>
       </c>
       <c r="V317" s="17" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="W317" s="18" t="s">
         <v>226</v>
@@ -15280,7 +15271,7 @@
       <c r="V351" s="34"/>
       <c r="W351" s="35"/>
     </row>
-    <row r="352" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:23" ht="156" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="10" t="s">
         <v>241</v>
       </c>
@@ -15344,8 +15335,8 @@
       <c r="U352" s="16">
         <v>80</v>
       </c>
-      <c r="V352" s="164" t="s">
-        <v>556</v>
+      <c r="V352" s="17" t="s">
+        <v>554</v>
       </c>
       <c r="W352" s="55"/>
     </row>
@@ -15449,7 +15440,7 @@
       <c r="V356" s="34"/>
       <c r="W356" s="35"/>
     </row>
-    <row r="357" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:23" ht="242.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="19"/>
       <c r="B357" s="11" t="s">
         <v>244</v>
@@ -15511,8 +15502,8 @@
       <c r="U357" s="16">
         <v>80</v>
       </c>
-      <c r="V357" s="164" t="s">
-        <v>557</v>
+      <c r="V357" s="17" t="s">
+        <v>555</v>
       </c>
       <c r="W357" s="55"/>
     </row>
@@ -15679,7 +15670,7 @@
         <v>80</v>
       </c>
       <c r="V362" s="17" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="W362" s="18" t="s">
         <v>243</v>
@@ -16799,7 +16790,7 @@
       <c r="V396" s="34"/>
       <c r="W396" s="35"/>
     </row>
-    <row r="397" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:23" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A397" s="19"/>
       <c r="B397" s="11" t="s">
         <v>265</v>
@@ -16861,8 +16852,8 @@
       <c r="U397" s="16">
         <v>80</v>
       </c>
-      <c r="V397" s="164" t="s">
-        <v>570</v>
+      <c r="V397" s="17" t="s">
+        <v>568</v>
       </c>
       <c r="W397" s="55"/>
     </row>
@@ -16968,7 +16959,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="402" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:23" ht="363" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A402" s="60"/>
       <c r="B402" s="61" t="s">
         <v>267</v>
@@ -17030,8 +17021,8 @@
       <c r="U402" s="66">
         <v>90</v>
       </c>
-      <c r="V402" s="164" t="s">
-        <v>559</v>
+      <c r="V402" s="67" t="s">
+        <v>557</v>
       </c>
       <c r="W402" s="83"/>
     </row>
@@ -17057,7 +17048,7 @@
       <c r="S403" s="72"/>
       <c r="T403" s="72"/>
       <c r="U403" s="72"/>
-      <c r="V403" s="94"/>
+      <c r="V403" s="92"/>
       <c r="W403" s="83"/>
     </row>
     <row r="404" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -17082,7 +17073,7 @@
       <c r="S404" s="72"/>
       <c r="T404" s="72"/>
       <c r="U404" s="72"/>
-      <c r="V404" s="94"/>
+      <c r="V404" s="92"/>
       <c r="W404" s="36" t="s">
         <v>268</v>
       </c>
@@ -17109,7 +17100,7 @@
       <c r="S405" s="72"/>
       <c r="T405" s="72"/>
       <c r="U405" s="72"/>
-      <c r="V405" s="94"/>
+      <c r="V405" s="92"/>
       <c r="W405" s="36" t="s">
         <v>269</v>
       </c>
@@ -17142,7 +17133,7 @@
     <row r="407" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A407" s="19"/>
       <c r="B407" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C407" s="12">
         <v>0</v>
@@ -17309,7 +17300,7 @@
     <row r="412" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A412" s="19"/>
       <c r="B412" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C412" s="12">
         <v>0</v>
@@ -17538,7 +17529,7 @@
         <v>90</v>
       </c>
       <c r="V417" s="17" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="W417" s="18" t="s">
         <v>274</v>
@@ -17651,7 +17642,7 @@
     <row r="422" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A422" s="19"/>
       <c r="B422" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C422" s="12">
         <v>0</v>
@@ -17711,7 +17702,7 @@
         <v>90</v>
       </c>
       <c r="V422" s="17" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="W422" s="18" t="s">
         <v>277</v>
@@ -18394,7 +18385,7 @@
       </c>
       <c r="V442" s="26"/>
       <c r="W442" s="18" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="443" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -18562,7 +18553,7 @@
         <v>100</v>
       </c>
       <c r="V447" s="17" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="W447" s="18" t="s">
         <v>293</v>
@@ -18900,7 +18891,7 @@
         <v>120</v>
       </c>
       <c r="V457" s="17" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="W457" s="18" t="s">
         <v>298</v>
@@ -19008,7 +18999,7 @@
       <c r="V461" s="34"/>
       <c r="W461" s="52"/>
     </row>
-    <row r="462" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:23" ht="225" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A462" s="10"/>
       <c r="B462" s="11" t="s">
         <v>300</v>
@@ -19061,15 +19052,19 @@
       <c r="R462" s="15">
         <v>8</v>
       </c>
-      <c r="S462" s="16"/>
-      <c r="T462" s="16"/>
-      <c r="U462" s="16"/>
+      <c r="S462" s="16">
+        <v>3</v>
+      </c>
+      <c r="T462" s="16">
+        <v>3</v>
+      </c>
+      <c r="U462" s="16">
+        <v>3</v>
+      </c>
       <c r="V462" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="W462" s="18" t="s">
-        <v>302</v>
-      </c>
+        <v>586</v>
+      </c>
+      <c r="W462" s="18"/>
     </row>
     <row r="463" spans="1:23" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A463" s="19"/>
@@ -19095,7 +19090,7 @@
       <c r="U463" s="25"/>
       <c r="V463" s="26"/>
       <c r="W463" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="464" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19175,10 +19170,10 @@
     </row>
     <row r="467" spans="1:23" ht="173.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A467" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B467" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C467" s="12">
         <v>0</v>
@@ -19238,10 +19233,10 @@
         <v>90</v>
       </c>
       <c r="V467" s="17" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="W467" s="18" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="468" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19268,7 +19263,7 @@
       <c r="U468" s="25"/>
       <c r="V468" s="26"/>
       <c r="W468" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="469" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19295,7 +19290,7 @@
       <c r="U469" s="25"/>
       <c r="V469" s="26"/>
       <c r="W469" s="18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="470" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19322,7 +19317,7 @@
       <c r="U470" s="25"/>
       <c r="V470" s="26"/>
       <c r="W470" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="471" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
@@ -19349,13 +19344,13 @@
       <c r="U471" s="33"/>
       <c r="V471" s="34"/>
       <c r="W471" s="52" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="472" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A472" s="19"/>
       <c r="B472" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C472" s="12">
         <v>0</v>
@@ -19519,8 +19514,8 @@
     </row>
     <row r="477" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A477" s="19"/>
-      <c r="B477" s="92" t="s">
-        <v>533</v>
+      <c r="B477" s="11" t="s">
+        <v>531</v>
       </c>
       <c r="C477" s="12">
         <v>0</v>
@@ -19581,7 +19576,7 @@
       </c>
       <c r="V477" s="26"/>
       <c r="W477" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="478" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19687,7 +19682,7 @@
     <row r="482" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A482" s="19"/>
       <c r="B482" s="20" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C482" s="12">
         <v>0</v>
@@ -19748,7 +19743,7 @@
       </c>
       <c r="V482" s="26"/>
       <c r="W482" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="483" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19760,11 +19755,11 @@
       <c r="F483" s="22"/>
       <c r="G483" s="22"/>
       <c r="H483" s="22"/>
-      <c r="I483" s="151"/>
-      <c r="J483" s="152"/>
-      <c r="K483" s="152"/>
-      <c r="L483" s="152"/>
-      <c r="M483" s="153"/>
+      <c r="I483" s="153"/>
+      <c r="J483" s="154"/>
+      <c r="K483" s="154"/>
+      <c r="L483" s="154"/>
+      <c r="M483" s="155"/>
       <c r="N483" s="24"/>
       <c r="O483" s="24"/>
       <c r="P483" s="24"/>
@@ -19854,7 +19849,7 @@
     <row r="487" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A487" s="19"/>
       <c r="B487" s="11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C487" s="12">
         <v>0</v>
@@ -19915,7 +19910,7 @@
       </c>
       <c r="V487" s="26"/>
       <c r="W487" s="18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="488" spans="1:23" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19942,7 +19937,7 @@
       <c r="U488" s="25"/>
       <c r="V488" s="26"/>
       <c r="W488" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="489" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -19969,7 +19964,7 @@
       <c r="U489" s="25"/>
       <c r="V489" s="26"/>
       <c r="W489" s="18" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="490" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -19996,7 +19991,7 @@
       <c r="U490" s="25"/>
       <c r="V490" s="26"/>
       <c r="W490" s="18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="491" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20023,13 +20018,13 @@
       <c r="U491" s="33"/>
       <c r="V491" s="34"/>
       <c r="W491" s="52" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="492" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A492" s="19"/>
       <c r="B492" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C492" s="12">
         <v>0</v>
@@ -20090,7 +20085,7 @@
       </c>
       <c r="V492" s="26"/>
       <c r="W492" s="18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="493" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20117,7 +20112,7 @@
       <c r="U493" s="25"/>
       <c r="V493" s="26"/>
       <c r="W493" s="18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="494" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20198,7 +20193,7 @@
     <row r="497" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A497" s="19"/>
       <c r="B497" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C497" s="12">
         <v>0</v>
@@ -20259,7 +20254,7 @@
       </c>
       <c r="V497" s="26"/>
       <c r="W497" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="498" spans="1:23" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20286,7 +20281,7 @@
       <c r="U498" s="25"/>
       <c r="V498" s="26"/>
       <c r="W498" s="18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="499" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20313,7 +20308,7 @@
       <c r="U499" s="25"/>
       <c r="V499" s="26"/>
       <c r="W499" s="18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="500" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20369,7 +20364,7 @@
     <row r="502" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A502" s="19"/>
       <c r="B502" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C502" s="12">
         <v>0</v>
@@ -20430,7 +20425,7 @@
       </c>
       <c r="V502" s="26"/>
       <c r="W502" s="18" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="503" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20457,7 +20452,7 @@
       <c r="U503" s="25"/>
       <c r="V503" s="26"/>
       <c r="W503" s="18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="504" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
@@ -20484,7 +20479,7 @@
       <c r="U504" s="25"/>
       <c r="V504" s="26"/>
       <c r="W504" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="505" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20540,7 +20535,7 @@
     <row r="507" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A507" s="19"/>
       <c r="B507" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C507" s="12">
         <v>0</v>
@@ -20601,7 +20596,7 @@
       </c>
       <c r="V507" s="26"/>
       <c r="W507" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="508" spans="1:23" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20628,7 +20623,7 @@
       <c r="U508" s="25"/>
       <c r="V508" s="26"/>
       <c r="W508" s="18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="509" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20708,10 +20703,10 @@
     </row>
     <row r="512" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A512" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B512" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C512" s="12">
         <v>0</v>
@@ -20762,19 +20757,19 @@
         <v>12</v>
       </c>
       <c r="S512" s="16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="T512" s="16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="U512" s="16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V512" s="17" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="W512" s="18" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="513" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20826,7 +20821,7 @@
       <c r="U514" s="25"/>
       <c r="V514" s="26"/>
       <c r="W514" s="18" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="515" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20853,7 +20848,7 @@
       <c r="U515" s="25"/>
       <c r="V515" s="26"/>
       <c r="W515" s="43" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="516" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20884,7 +20879,7 @@
     <row r="517" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A517" s="10"/>
       <c r="B517" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C517" s="12">
         <v>0</v>
@@ -20945,7 +20940,7 @@
       </c>
       <c r="V517" s="26"/>
       <c r="W517" s="18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="518" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -20972,7 +20967,7 @@
       <c r="U518" s="25"/>
       <c r="V518" s="26"/>
       <c r="W518" s="18" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="519" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -20999,7 +20994,7 @@
       <c r="U519" s="25"/>
       <c r="V519" s="26"/>
       <c r="W519" s="18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="520" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21055,7 +21050,7 @@
     <row r="522" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A522" s="19"/>
       <c r="B522" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C522" s="12">
         <v>0</v>
@@ -21094,13 +21089,13 @@
         <v>26</v>
       </c>
       <c r="O522" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P522" s="15">
         <v>23</v>
       </c>
       <c r="Q522" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="R522" s="15">
         <v>20</v>
@@ -21115,10 +21110,10 @@
         <v>120</v>
       </c>
       <c r="V522" s="17" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="W522" s="18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="523" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21170,7 +21165,7 @@
       <c r="U524" s="25"/>
       <c r="V524" s="26"/>
       <c r="W524" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="525" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21226,7 +21221,7 @@
     <row r="527" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A527" s="19"/>
       <c r="B527" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C527" s="82">
         <v>0</v>
@@ -21391,7 +21386,7 @@
     <row r="532" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A532" s="19"/>
       <c r="B532" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C532" s="12">
         <v>0</v>
@@ -21451,10 +21446,10 @@
         <v>80</v>
       </c>
       <c r="V532" s="17" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="W532" s="18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="533" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21481,7 +21476,7 @@
       <c r="U533" s="25"/>
       <c r="V533" s="26"/>
       <c r="W533" s="18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="534" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21559,10 +21554,10 @@
       <c r="V536" s="34"/>
       <c r="W536" s="35"/>
     </row>
-    <row r="537" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:23" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A537" s="19"/>
       <c r="B537" s="11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C537" s="12">
         <v>0</v>
@@ -21621,8 +21616,8 @@
       <c r="U537" s="16">
         <v>160</v>
       </c>
-      <c r="V537" s="164" t="s">
-        <v>576</v>
+      <c r="V537" s="17" t="s">
+        <v>573</v>
       </c>
       <c r="W537" s="18"/>
     </row>
@@ -21729,7 +21724,7 @@
     <row r="542" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A542" s="19"/>
       <c r="B542" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C542" s="12">
         <v>0</v>
@@ -21784,7 +21779,7 @@
       <c r="U542" s="16"/>
       <c r="V542" s="26"/>
       <c r="W542" s="18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="543" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21890,18 +21885,18 @@
     <row r="547" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A547" s="19"/>
       <c r="B547" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C547" s="12">
         <v>0</v>
       </c>
-      <c r="D547" s="154" t="s">
-        <v>356</v>
-      </c>
-      <c r="E547" s="155"/>
-      <c r="F547" s="155"/>
-      <c r="G547" s="155"/>
-      <c r="H547" s="156"/>
+      <c r="D547" s="156" t="s">
+        <v>354</v>
+      </c>
+      <c r="E547" s="157"/>
+      <c r="F547" s="157"/>
+      <c r="G547" s="157"/>
+      <c r="H547" s="158"/>
       <c r="I547" s="14">
         <v>17</v>
       </c>
@@ -21942,10 +21937,10 @@
         <v>100</v>
       </c>
       <c r="V547" s="17" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="W547" s="18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="548" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.3">
@@ -21972,7 +21967,7 @@
       <c r="U548" s="25"/>
       <c r="V548" s="26"/>
       <c r="W548" s="18" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="549" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22053,7 +22048,7 @@
     <row r="552" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A552" s="19"/>
       <c r="B552" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C552" s="12">
         <v>0</v>
@@ -22218,7 +22213,7 @@
     <row r="557" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A557" s="19"/>
       <c r="B557" s="11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C557" s="12">
         <v>0</v>
@@ -22383,7 +22378,7 @@
     <row r="562" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A562" s="19"/>
       <c r="B562" s="11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C562" s="12">
         <v>0</v>
@@ -22444,7 +22439,7 @@
       </c>
       <c r="V562" s="26"/>
       <c r="W562" s="18" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="563" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22471,7 +22466,7 @@
       <c r="U563" s="25"/>
       <c r="V563" s="26"/>
       <c r="W563" s="18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="564" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -22498,7 +22493,7 @@
       <c r="U564" s="25"/>
       <c r="V564" s="26"/>
       <c r="W564" s="36" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="565" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22525,7 +22520,7 @@
       <c r="U565" s="25"/>
       <c r="V565" s="26"/>
       <c r="W565" s="18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="566" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -22552,13 +22547,13 @@
       <c r="U566" s="33"/>
       <c r="V566" s="34"/>
       <c r="W566" s="52" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="567" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="567" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A567" s="19"/>
       <c r="B567" s="11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C567" s="12">
         <v>0</v>
@@ -22567,41 +22562,47 @@
         <v>8</v>
       </c>
       <c r="E567" s="13">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="F567" s="13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G567" s="13">
-        <v>4.8</v>
-      </c>
-      <c r="H567" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="H567" s="13">
+        <v>8</v>
+      </c>
       <c r="I567" s="14">
         <v>10</v>
       </c>
       <c r="J567" s="14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K567" s="14">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="L567" s="14">
-        <v>6</v>
-      </c>
-      <c r="M567" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="M567" s="14">
+        <v>10</v>
+      </c>
       <c r="N567" s="15">
         <v>12</v>
       </c>
       <c r="O567" s="15">
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="P567" s="15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q567" s="15">
-        <v>7.2</v>
-      </c>
-      <c r="R567" s="15"/>
+        <v>12</v>
+      </c>
+      <c r="R567" s="15">
+        <v>12</v>
+      </c>
       <c r="S567" s="16">
         <v>140</v>
       </c>
@@ -22611,9 +22612,11 @@
       <c r="U567" s="16">
         <v>100</v>
       </c>
-      <c r="V567" s="26"/>
+      <c r="V567" s="162" t="s">
+        <v>587</v>
+      </c>
       <c r="W567" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="568" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22719,7 +22722,7 @@
     <row r="572" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A572" s="19"/>
       <c r="B572" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C572" s="12">
         <v>0</v>
@@ -22884,7 +22887,7 @@
     <row r="577" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A577" s="19"/>
       <c r="B577" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C577" s="12">
         <v>0</v>
@@ -22944,10 +22947,10 @@
         <v>120</v>
       </c>
       <c r="V577" s="17" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="W577" s="18" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="578" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23053,7 +23056,7 @@
     <row r="582" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A582" s="19"/>
       <c r="B582" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C582" s="12">
         <v>0</v>
@@ -23114,7 +23117,7 @@
       </c>
       <c r="V582" s="26"/>
       <c r="W582" s="18" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="583" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23166,7 +23169,7 @@
       <c r="U584" s="25"/>
       <c r="V584" s="26"/>
       <c r="W584" s="18" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="585" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23222,7 +23225,7 @@
     <row r="587" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A587" s="19"/>
       <c r="B587" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C587" s="12">
         <v>0</v>
@@ -23386,10 +23389,10 @@
     </row>
     <row r="592" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A592" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B592" s="11" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C592" s="12">
         <v>0</v>
@@ -23450,7 +23453,7 @@
       </c>
       <c r="V592" s="26"/>
       <c r="W592" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="593" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23502,7 +23505,7 @@
       <c r="U594" s="25"/>
       <c r="V594" s="26"/>
       <c r="W594" s="85" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="595" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23529,7 +23532,7 @@
       <c r="U595" s="25"/>
       <c r="V595" s="26"/>
       <c r="W595" s="18" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="596" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
@@ -23556,13 +23559,13 @@
       <c r="U596" s="33"/>
       <c r="V596" s="34"/>
       <c r="W596" s="52" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="597" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A597" s="19"/>
       <c r="B597" s="11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C597" s="12">
         <v>0</v>
@@ -23622,10 +23625,10 @@
         <v>120</v>
       </c>
       <c r="V597" s="17" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="W597" s="56" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="598" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23702,7 +23705,7 @@
       <c r="U600" s="25"/>
       <c r="V600" s="26"/>
       <c r="W600" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="601" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23729,13 +23732,13 @@
       <c r="U601" s="33"/>
       <c r="V601" s="34"/>
       <c r="W601" s="52" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="602" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A602" s="19"/>
       <c r="B602" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C602" s="12">
         <v>0</v>
@@ -23796,7 +23799,7 @@
       </c>
       <c r="V602" s="26"/>
       <c r="W602" s="18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="603" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23848,7 +23851,7 @@
       <c r="U604" s="25"/>
       <c r="V604" s="26"/>
       <c r="W604" s="18" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="605" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -23875,7 +23878,7 @@
       <c r="U605" s="25"/>
       <c r="V605" s="26"/>
       <c r="W605" s="18" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="606" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23906,7 +23909,7 @@
     <row r="607" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A607" s="19"/>
       <c r="B607" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C607" s="12">
         <v>0</v>
@@ -23967,7 +23970,7 @@
       </c>
       <c r="V607" s="26"/>
       <c r="W607" s="18" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="608" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -23994,7 +23997,7 @@
       <c r="U608" s="25"/>
       <c r="V608" s="26"/>
       <c r="W608" s="18" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="609" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24021,7 +24024,7 @@
       <c r="U609" s="25"/>
       <c r="V609" s="26"/>
       <c r="W609" s="18" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="610" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24048,7 +24051,7 @@
       <c r="U610" s="25"/>
       <c r="V610" s="26"/>
       <c r="W610" s="18" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="611" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24079,7 +24082,7 @@
     <row r="612" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A612" s="19"/>
       <c r="B612" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C612" s="12">
         <v>0</v>
@@ -24114,11 +24117,21 @@
       <c r="M612" s="14">
         <v>17</v>
       </c>
-      <c r="N612" s="15"/>
-      <c r="O612" s="15"/>
-      <c r="P612" s="15"/>
-      <c r="Q612" s="15"/>
-      <c r="R612" s="15"/>
+      <c r="N612" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O612" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P612" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q612" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R612" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="S612" s="16">
         <v>30</v>
       </c>
@@ -24130,7 +24143,7 @@
       </c>
       <c r="V612" s="26"/>
       <c r="W612" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="613" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -24157,7 +24170,7 @@
       <c r="U613" s="25"/>
       <c r="V613" s="26"/>
       <c r="W613" s="18" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="614" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24238,7 +24251,7 @@
     <row r="617" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A617" s="19"/>
       <c r="B617" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C617" s="12">
         <v>0</v>
@@ -24299,7 +24312,7 @@
       </c>
       <c r="V617" s="26"/>
       <c r="W617" s="18" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="618" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24405,7 +24418,7 @@
     <row r="622" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A622" s="19"/>
       <c r="B622" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C622" s="12">
         <v>0</v>
@@ -24466,7 +24479,7 @@
       </c>
       <c r="V622" s="26"/>
       <c r="W622" s="18" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="623" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -24493,7 +24506,7 @@
       <c r="U623" s="25"/>
       <c r="V623" s="26"/>
       <c r="W623" s="18" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="624" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24574,7 +24587,7 @@
     <row r="627" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A627" s="19"/>
       <c r="B627" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C627" s="12">
         <v>0</v>
@@ -24739,7 +24752,7 @@
     <row r="632" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A632" s="19"/>
       <c r="B632" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C632" s="12">
         <v>0</v>
@@ -24800,7 +24813,7 @@
       </c>
       <c r="V632" s="26"/>
       <c r="W632" s="18" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="633" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24827,7 +24840,7 @@
       <c r="U633" s="25"/>
       <c r="V633" s="26"/>
       <c r="W633" s="18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="634" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24908,7 +24921,7 @@
     <row r="637" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A637" s="19"/>
       <c r="B637" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C637" s="12">
         <v>0</v>
@@ -24943,11 +24956,21 @@
       <c r="M637" s="14">
         <v>6</v>
       </c>
-      <c r="N637" s="15"/>
-      <c r="O637" s="15"/>
-      <c r="P637" s="15"/>
-      <c r="Q637" s="15"/>
-      <c r="R637" s="15"/>
+      <c r="N637" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O637" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P637" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q637" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R637" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="S637" s="16">
         <v>180</v>
       </c>
@@ -25063,7 +25086,7 @@
     <row r="642" spans="1:23" ht="263.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A642" s="19"/>
       <c r="B642" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C642" s="12">
         <v>0</v>
@@ -25124,7 +25147,7 @@
       </c>
       <c r="V642" s="26"/>
       <c r="W642" s="18" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="643" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.3">
@@ -25151,7 +25174,7 @@
       <c r="U643" s="25"/>
       <c r="V643" s="26"/>
       <c r="W643" s="18" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="644" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25231,10 +25254,10 @@
     </row>
     <row r="647" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A647" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B647" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C647" s="12">
         <v>0</v>
@@ -25294,10 +25317,10 @@
         <v>6</v>
       </c>
       <c r="V647" s="16" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="W647" s="18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="648" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25324,7 +25347,7 @@
       <c r="U648" s="25"/>
       <c r="V648" s="25"/>
       <c r="W648" s="18" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="649" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25376,7 +25399,7 @@
       <c r="U650" s="25"/>
       <c r="V650" s="25"/>
       <c r="W650" s="18" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="651" spans="1:23" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25403,13 +25426,13 @@
       <c r="U651" s="33"/>
       <c r="V651" s="51"/>
       <c r="W651" s="35" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="652" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="652" spans="1:23" ht="294" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A652" s="19"/>
       <c r="B652" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C652" s="12">
         <v>0</v>
@@ -25448,7 +25471,7 @@
         <v>16</v>
       </c>
       <c r="O652" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P652" s="15">
         <v>15</v>
@@ -25468,8 +25491,8 @@
       <c r="U652" s="16">
         <v>70</v>
       </c>
-      <c r="V652" s="164" t="s">
-        <v>581</v>
+      <c r="V652" s="17" t="s">
+        <v>578</v>
       </c>
       <c r="W652" s="18"/>
     </row>
@@ -25575,10 +25598,10 @@
     </row>
     <row r="657" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A657" s="10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B657" s="11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C657" s="12">
         <v>0</v>
@@ -25664,7 +25687,7 @@
       <c r="U658" s="25"/>
       <c r="V658" s="26"/>
       <c r="W658" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="659" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25691,7 +25714,7 @@
       <c r="U659" s="25"/>
       <c r="V659" s="26"/>
       <c r="W659" s="18" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="660" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25718,7 +25741,7 @@
       <c r="U660" s="25"/>
       <c r="V660" s="26"/>
       <c r="W660" s="18" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="661" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25749,7 +25772,7 @@
     <row r="662" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A662" s="19"/>
       <c r="B662" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C662" s="12">
         <v>0</v>
@@ -25769,11 +25792,21 @@
       <c r="H662" s="13">
         <v>2</v>
       </c>
-      <c r="I662" s="14"/>
-      <c r="J662" s="14"/>
-      <c r="K662" s="14"/>
-      <c r="L662" s="14"/>
-      <c r="M662" s="14"/>
+      <c r="I662" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J662" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K662" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L662" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="M662" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="N662" s="15">
         <v>20</v>
       </c>
@@ -25800,7 +25833,7 @@
       </c>
       <c r="V662" s="26"/>
       <c r="W662" s="18" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="663" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25827,7 +25860,7 @@
       <c r="U663" s="25"/>
       <c r="V663" s="26"/>
       <c r="W663" s="18" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="664" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -25854,7 +25887,7 @@
       <c r="U664" s="25"/>
       <c r="V664" s="26"/>
       <c r="W664" s="18" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="665" spans="1:23" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -25881,7 +25914,7 @@
       <c r="U665" s="25"/>
       <c r="V665" s="26"/>
       <c r="W665" s="18" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="666" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25908,13 +25941,13 @@
       <c r="U666" s="33"/>
       <c r="V666" s="34"/>
       <c r="W666" s="52" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="667" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A667" s="19"/>
       <c r="B667" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C667" s="12">
         <v>0</v>
@@ -25975,7 +26008,7 @@
       </c>
       <c r="V667" s="26"/>
       <c r="W667" s="18" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="668" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.3">
@@ -26002,7 +26035,7 @@
       <c r="U668" s="25"/>
       <c r="V668" s="26"/>
       <c r="W668" s="18" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="669" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.3">
@@ -26029,7 +26062,7 @@
       <c r="U669" s="25"/>
       <c r="V669" s="26"/>
       <c r="W669" s="18" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="670" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.3">
@@ -26056,7 +26089,7 @@
       <c r="U670" s="25"/>
       <c r="V670" s="26"/>
       <c r="W670" s="18" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="671" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.3">
@@ -26083,13 +26116,13 @@
       <c r="U671" s="33"/>
       <c r="V671" s="34"/>
       <c r="W671" s="52" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="672" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A672" s="19"/>
       <c r="B672" s="11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C672" s="12">
         <v>0</v>
@@ -26152,7 +26185,7 @@
         <v>0</v>
       </c>
       <c r="W672" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="673" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -26258,7 +26291,7 @@
     <row r="677" spans="1:23" ht="173.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A677" s="19"/>
       <c r="B677" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C677" s="12">
         <v>0</v>
@@ -26278,11 +26311,21 @@
       <c r="H677" s="13">
         <v>6</v>
       </c>
-      <c r="I677" s="14"/>
-      <c r="J677" s="14"/>
-      <c r="K677" s="14"/>
-      <c r="L677" s="14"/>
-      <c r="M677" s="14"/>
+      <c r="I677" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J677" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K677" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L677" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="M677" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="N677" s="15">
         <v>14</v>
       </c>
@@ -26308,10 +26351,10 @@
         <v>80</v>
       </c>
       <c r="V677" s="17" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="W677" s="18" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="678" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -26338,7 +26381,7 @@
       <c r="U678" s="25"/>
       <c r="V678" s="26"/>
       <c r="W678" s="18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="679" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -26419,7 +26462,7 @@
     <row r="682" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A682" s="19"/>
       <c r="B682" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C682" s="12">
         <v>0</v>
@@ -26584,7 +26627,7 @@
     <row r="687" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A687" s="19"/>
       <c r="B687" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C687" s="12">
         <v>0</v>
@@ -26749,7 +26792,7 @@
     <row r="692" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A692" s="19"/>
       <c r="B692" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C692" s="12">
         <v>0</v>
@@ -26810,7 +26853,7 @@
       </c>
       <c r="V692" s="17"/>
       <c r="W692" s="18" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="693" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -26837,7 +26880,7 @@
       <c r="U693" s="25"/>
       <c r="V693" s="26"/>
       <c r="W693" s="18" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="694" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -26864,7 +26907,7 @@
       <c r="U694" s="25"/>
       <c r="V694" s="26"/>
       <c r="W694" s="18" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="695" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -26919,10 +26962,10 @@
     </row>
     <row r="697" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A697" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B697" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C697" s="12">
         <v>0</v>
@@ -26983,7 +27026,7 @@
       </c>
       <c r="V697" s="26"/>
       <c r="W697" s="18" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="698" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27089,7 +27132,7 @@
     <row r="702" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A702" s="19"/>
       <c r="B702" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C702" s="12">
         <v>0</v>
@@ -27253,10 +27296,10 @@
     </row>
     <row r="707" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A707" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B707" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C707" s="12">
         <v>0</v>
@@ -27317,7 +27360,7 @@
       </c>
       <c r="V707" s="26"/>
       <c r="W707" s="18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="708" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27344,7 +27387,7 @@
       <c r="U708" s="25"/>
       <c r="V708" s="26"/>
       <c r="W708" s="18" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="709" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27425,7 +27468,7 @@
     <row r="712" spans="1:23" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A712" s="19"/>
       <c r="B712" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C712" s="12">
         <v>0</v>
@@ -27485,10 +27528,10 @@
         <v>100</v>
       </c>
       <c r="V712" s="17" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="W712" s="18" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="713" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27515,7 +27558,7 @@
       <c r="U713" s="25"/>
       <c r="V713" s="26"/>
       <c r="W713" s="18" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="714" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -27542,7 +27585,7 @@
       <c r="U714" s="25"/>
       <c r="V714" s="26"/>
       <c r="W714" s="18" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="715" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27598,7 +27641,7 @@
     <row r="717" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A717" s="19"/>
       <c r="B717" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C717" s="12">
         <v>0</v>
@@ -27659,10 +27702,10 @@
       </c>
       <c r="V717" s="26"/>
       <c r="W717" s="18" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="718" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="718" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A718" s="19"/>
       <c r="B718" s="20"/>
       <c r="C718" s="21"/>
@@ -27685,8 +27728,8 @@
       <c r="T718" s="25"/>
       <c r="U718" s="25"/>
       <c r="V718" s="26"/>
-      <c r="W718" s="86" t="s">
-        <v>461</v>
+      <c r="W718" s="18" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="719" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27766,10 +27809,10 @@
     </row>
     <row r="722" spans="1:23" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A722" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B722" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C722" s="12">
         <v>0</v>
@@ -27777,12 +27820,12 @@
       <c r="D722" s="13">
         <v>4</v>
       </c>
-      <c r="E722" s="154" t="s">
-        <v>464</v>
-      </c>
-      <c r="F722" s="155"/>
-      <c r="G722" s="155"/>
-      <c r="H722" s="156"/>
+      <c r="E722" s="156" t="s">
+        <v>462</v>
+      </c>
+      <c r="F722" s="157"/>
+      <c r="G722" s="157"/>
+      <c r="H722" s="158"/>
       <c r="I722" s="14">
         <v>30</v>
       </c>
@@ -27799,19 +27842,19 @@
         <v>18</v>
       </c>
       <c r="N722" s="15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O722" s="15" t="s">
+        <v>463</v>
+      </c>
+      <c r="P722" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q722" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="P722" s="15" t="s">
+      <c r="R722" s="15" t="s">
         <v>466</v>
-      </c>
-      <c r="Q722" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="R722" s="15" t="s">
-        <v>468</v>
       </c>
       <c r="S722" s="16">
         <v>80</v>
@@ -27824,42 +27867,42 @@
       </c>
       <c r="V722" s="26"/>
       <c r="W722" s="18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="723" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A723" s="19"/>
       <c r="B723" s="20"/>
       <c r="C723" s="21"/>
-      <c r="D723" s="105" t="s">
-        <v>470</v>
-      </c>
-      <c r="E723" s="106"/>
-      <c r="F723" s="106"/>
-      <c r="G723" s="106"/>
-      <c r="H723" s="107"/>
+      <c r="D723" s="107" t="s">
+        <v>468</v>
+      </c>
+      <c r="E723" s="108"/>
+      <c r="F723" s="108"/>
+      <c r="G723" s="108"/>
+      <c r="H723" s="109"/>
       <c r="I723" s="23">
         <v>27</v>
       </c>
       <c r="J723" s="23" t="s">
+        <v>469</v>
+      </c>
+      <c r="K723" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="L723" s="23" t="s">
         <v>471</v>
       </c>
-      <c r="K723" s="23" t="s">
+      <c r="M723" s="23" t="s">
         <v>472</v>
       </c>
-      <c r="L723" s="23" t="s">
+      <c r="N723" s="159" t="s">
         <v>473</v>
       </c>
-      <c r="M723" s="23" t="s">
-        <v>474</v>
-      </c>
-      <c r="N723" s="157" t="s">
-        <v>475</v>
-      </c>
-      <c r="O723" s="158"/>
-      <c r="P723" s="158"/>
-      <c r="Q723" s="158"/>
-      <c r="R723" s="159"/>
+      <c r="O723" s="160"/>
+      <c r="P723" s="160"/>
+      <c r="Q723" s="160"/>
+      <c r="R723" s="161"/>
       <c r="S723" s="25">
         <v>72</v>
       </c>
@@ -27876,25 +27919,25 @@
       <c r="A724" s="19"/>
       <c r="B724" s="20"/>
       <c r="C724" s="21"/>
-      <c r="D724" s="108"/>
-      <c r="E724" s="109"/>
-      <c r="F724" s="109"/>
-      <c r="G724" s="109"/>
-      <c r="H724" s="110"/>
+      <c r="D724" s="110"/>
+      <c r="E724" s="111"/>
+      <c r="F724" s="111"/>
+      <c r="G724" s="111"/>
+      <c r="H724" s="112"/>
       <c r="I724" s="23">
         <v>24</v>
       </c>
       <c r="J724" s="23" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K724" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="L724" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="M724" s="23" t="s">
         <v>476</v>
-      </c>
-      <c r="L724" s="23" t="s">
-        <v>477</v>
-      </c>
-      <c r="M724" s="23" t="s">
-        <v>478</v>
       </c>
       <c r="N724" s="24"/>
       <c r="O724" s="24"/>
@@ -27917,25 +27960,25 @@
       <c r="A725" s="19"/>
       <c r="B725" s="20"/>
       <c r="C725" s="21"/>
-      <c r="D725" s="111"/>
-      <c r="E725" s="112"/>
-      <c r="F725" s="112"/>
-      <c r="G725" s="112"/>
-      <c r="H725" s="113"/>
+      <c r="D725" s="113"/>
+      <c r="E725" s="114"/>
+      <c r="F725" s="114"/>
+      <c r="G725" s="114"/>
+      <c r="H725" s="115"/>
       <c r="I725" s="23">
         <v>21</v>
       </c>
       <c r="J725" s="23" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K725" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="L725" s="23" t="s">
         <v>477</v>
       </c>
-      <c r="L725" s="23" t="s">
-        <v>479</v>
-      </c>
       <c r="M725" s="23" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="N725" s="71">
         <v>10</v>
@@ -27968,37 +28011,37 @@
       <c r="A726" s="27"/>
       <c r="B726" s="28"/>
       <c r="C726" s="29"/>
-      <c r="D726" s="123" t="s">
-        <v>481</v>
-      </c>
-      <c r="E726" s="124"/>
-      <c r="F726" s="124"/>
-      <c r="G726" s="125"/>
+      <c r="D726" s="125" t="s">
+        <v>479</v>
+      </c>
+      <c r="E726" s="126"/>
+      <c r="F726" s="126"/>
+      <c r="G726" s="127"/>
       <c r="H726" s="30" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I726" s="31">
         <v>18</v>
       </c>
       <c r="J726" s="31" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K726" s="31" t="s">
+        <v>476</v>
+      </c>
+      <c r="L726" s="31" t="s">
         <v>478</v>
       </c>
-      <c r="L726" s="31" t="s">
-        <v>480</v>
-      </c>
       <c r="M726" s="31" t="s">
-        <v>483</v>
-      </c>
-      <c r="N726" s="129" t="s">
-        <v>484</v>
-      </c>
-      <c r="O726" s="130"/>
-      <c r="P726" s="130"/>
-      <c r="Q726" s="130"/>
-      <c r="R726" s="131"/>
+        <v>481</v>
+      </c>
+      <c r="N726" s="131" t="s">
+        <v>482</v>
+      </c>
+      <c r="O726" s="132"/>
+      <c r="P726" s="132"/>
+      <c r="Q726" s="132"/>
+      <c r="R726" s="133"/>
       <c r="S726" s="51">
         <v>48</v>
       </c>
@@ -28014,7 +28057,7 @@
     <row r="727" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A727" s="19"/>
       <c r="B727" s="20" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C727" s="12">
         <v>0</v>
@@ -28022,21 +28065,21 @@
       <c r="D727" s="22">
         <v>4</v>
       </c>
-      <c r="E727" s="99" t="s">
-        <v>464</v>
-      </c>
-      <c r="F727" s="100"/>
-      <c r="G727" s="100"/>
-      <c r="H727" s="101"/>
+      <c r="E727" s="101" t="s">
+        <v>462</v>
+      </c>
+      <c r="F727" s="102"/>
+      <c r="G727" s="102"/>
+      <c r="H727" s="103"/>
       <c r="I727" s="23">
         <v>16</v>
       </c>
-      <c r="J727" s="102" t="s">
-        <v>464</v>
-      </c>
-      <c r="K727" s="103"/>
-      <c r="L727" s="103"/>
-      <c r="M727" s="104"/>
+      <c r="J727" s="104" t="s">
+        <v>462</v>
+      </c>
+      <c r="K727" s="105"/>
+      <c r="L727" s="105"/>
+      <c r="M727" s="106"/>
       <c r="N727" s="24">
         <v>22</v>
       </c>
@@ -28063,38 +28106,38 @@
       </c>
       <c r="V727" s="26"/>
       <c r="W727" s="18" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="728" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A728" s="19"/>
       <c r="B728" s="20"/>
       <c r="C728" s="21"/>
-      <c r="D728" s="105" t="s">
-        <v>470</v>
-      </c>
-      <c r="E728" s="106"/>
-      <c r="F728" s="106"/>
-      <c r="G728" s="106"/>
-      <c r="H728" s="107"/>
-      <c r="I728" s="114" t="s">
-        <v>470</v>
-      </c>
-      <c r="J728" s="115"/>
-      <c r="K728" s="115"/>
-      <c r="L728" s="115"/>
-      <c r="M728" s="116"/>
+      <c r="D728" s="107" t="s">
+        <v>468</v>
+      </c>
+      <c r="E728" s="108"/>
+      <c r="F728" s="108"/>
+      <c r="G728" s="108"/>
+      <c r="H728" s="109"/>
+      <c r="I728" s="116" t="s">
+        <v>468</v>
+      </c>
+      <c r="J728" s="117"/>
+      <c r="K728" s="117"/>
+      <c r="L728" s="117"/>
+      <c r="M728" s="118"/>
       <c r="N728" s="24" t="s">
+        <v>485</v>
+      </c>
+      <c r="O728" s="24" t="s">
+        <v>486</v>
+      </c>
+      <c r="P728" s="24" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q728" s="24" t="s">
         <v>487</v>
-      </c>
-      <c r="O728" s="24" t="s">
-        <v>488</v>
-      </c>
-      <c r="P728" s="24" t="s">
-        <v>478</v>
-      </c>
-      <c r="Q728" s="24" t="s">
-        <v>489</v>
       </c>
       <c r="R728" s="24">
         <v>9</v>
@@ -28115,27 +28158,27 @@
       <c r="A729" s="19"/>
       <c r="B729" s="20"/>
       <c r="C729" s="21"/>
-      <c r="D729" s="108"/>
-      <c r="E729" s="109"/>
-      <c r="F729" s="109"/>
-      <c r="G729" s="109"/>
-      <c r="H729" s="110"/>
-      <c r="I729" s="117"/>
-      <c r="J729" s="118"/>
-      <c r="K729" s="118"/>
-      <c r="L729" s="118"/>
-      <c r="M729" s="119"/>
+      <c r="D729" s="110"/>
+      <c r="E729" s="111"/>
+      <c r="F729" s="111"/>
+      <c r="G729" s="111"/>
+      <c r="H729" s="112"/>
+      <c r="I729" s="119"/>
+      <c r="J729" s="120"/>
+      <c r="K729" s="120"/>
+      <c r="L729" s="120"/>
+      <c r="M729" s="121"/>
       <c r="N729" s="24" t="s">
+        <v>488</v>
+      </c>
+      <c r="O729" s="24" t="s">
+        <v>489</v>
+      </c>
+      <c r="P729" s="24" t="s">
         <v>490</v>
       </c>
-      <c r="O729" s="24" t="s">
+      <c r="Q729" s="24" t="s">
         <v>491</v>
-      </c>
-      <c r="P729" s="24" t="s">
-        <v>492</v>
-      </c>
-      <c r="Q729" s="24" t="s">
-        <v>493</v>
       </c>
       <c r="R729" s="24">
         <v>8</v>
@@ -28156,27 +28199,27 @@
       <c r="A730" s="19"/>
       <c r="B730" s="20"/>
       <c r="C730" s="21"/>
-      <c r="D730" s="111"/>
-      <c r="E730" s="112"/>
-      <c r="F730" s="112"/>
-      <c r="G730" s="112"/>
-      <c r="H730" s="113"/>
-      <c r="I730" s="120"/>
-      <c r="J730" s="121"/>
-      <c r="K730" s="121"/>
-      <c r="L730" s="121"/>
-      <c r="M730" s="122"/>
+      <c r="D730" s="113"/>
+      <c r="E730" s="114"/>
+      <c r="F730" s="114"/>
+      <c r="G730" s="114"/>
+      <c r="H730" s="115"/>
+      <c r="I730" s="122"/>
+      <c r="J730" s="123"/>
+      <c r="K730" s="123"/>
+      <c r="L730" s="123"/>
+      <c r="M730" s="124"/>
       <c r="N730" s="24" t="s">
+        <v>492</v>
+      </c>
+      <c r="O730" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="P730" s="24" t="s">
         <v>494</v>
       </c>
-      <c r="O730" s="24" t="s">
+      <c r="Q730" s="24" t="s">
         <v>495</v>
-      </c>
-      <c r="P730" s="24" t="s">
-        <v>496</v>
-      </c>
-      <c r="Q730" s="24" t="s">
-        <v>497</v>
       </c>
       <c r="R730" s="24">
         <v>7</v>
@@ -28197,35 +28240,35 @@
       <c r="A731" s="27"/>
       <c r="B731" s="28"/>
       <c r="C731" s="29"/>
-      <c r="D731" s="123" t="s">
-        <v>481</v>
-      </c>
-      <c r="E731" s="124"/>
-      <c r="F731" s="124"/>
-      <c r="G731" s="125"/>
+      <c r="D731" s="125" t="s">
+        <v>479</v>
+      </c>
+      <c r="E731" s="126"/>
+      <c r="F731" s="126"/>
+      <c r="G731" s="127"/>
       <c r="H731" s="30" t="s">
-        <v>482</v>
-      </c>
-      <c r="I731" s="126" t="s">
-        <v>498</v>
-      </c>
-      <c r="J731" s="127"/>
-      <c r="K731" s="127"/>
-      <c r="L731" s="128"/>
+        <v>480</v>
+      </c>
+      <c r="I731" s="128" t="s">
+        <v>496</v>
+      </c>
+      <c r="J731" s="129"/>
+      <c r="K731" s="129"/>
+      <c r="L731" s="130"/>
       <c r="M731" s="31">
         <v>6</v>
       </c>
       <c r="N731" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="O731" s="32" t="s">
+        <v>498</v>
+      </c>
+      <c r="P731" s="32" t="s">
         <v>499</v>
       </c>
-      <c r="O731" s="32" t="s">
+      <c r="Q731" s="32" t="s">
         <v>500</v>
-      </c>
-      <c r="P731" s="32" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q731" s="32" t="s">
-        <v>502</v>
       </c>
       <c r="R731" s="32">
         <v>6</v>
@@ -28245,7 +28288,7 @@
     <row r="732" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A732" s="19"/>
       <c r="B732" s="11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C732" s="12">
         <v>0</v>
@@ -28410,7 +28453,7 @@
     <row r="737" spans="1:23" ht="173.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A737" s="19"/>
       <c r="B737" s="11" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C737" s="12">
         <v>0</v>
@@ -28442,8 +28485,8 @@
       <c r="L737" s="14">
         <v>0</v>
       </c>
-      <c r="M737" s="87" t="s">
-        <v>505</v>
+      <c r="M737" s="86" t="s">
+        <v>503</v>
       </c>
       <c r="N737" s="15">
         <v>12</v>
@@ -28470,9 +28513,9 @@
         <v>90</v>
       </c>
       <c r="V737" s="17" t="s">
-        <v>586</v>
-      </c>
-      <c r="W737" s="88" t="s">
+        <v>583</v>
+      </c>
+      <c r="W737" s="87" t="s">
         <v>47</v>
       </c>
     </row>
@@ -28489,7 +28532,7 @@
       <c r="J738" s="23"/>
       <c r="K738" s="23"/>
       <c r="L738" s="23"/>
-      <c r="M738" s="89"/>
+      <c r="M738" s="88"/>
       <c r="N738" s="24"/>
       <c r="O738" s="24"/>
       <c r="P738" s="24"/>
@@ -28514,7 +28557,7 @@
       <c r="J739" s="23"/>
       <c r="K739" s="23"/>
       <c r="L739" s="23"/>
-      <c r="M739" s="89"/>
+      <c r="M739" s="88"/>
       <c r="N739" s="24"/>
       <c r="O739" s="24"/>
       <c r="P739" s="24"/>
@@ -28524,8 +28567,8 @@
       <c r="T739" s="25"/>
       <c r="U739" s="25"/>
       <c r="V739" s="26"/>
-      <c r="W739" s="90" t="s">
-        <v>506</v>
+      <c r="W739" s="89" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="740" spans="1:23" ht="156" thickBot="1" x14ac:dyDescent="0.3">
@@ -28541,7 +28584,7 @@
       <c r="J740" s="23"/>
       <c r="K740" s="23"/>
       <c r="L740" s="23"/>
-      <c r="M740" s="89"/>
+      <c r="M740" s="88"/>
       <c r="N740" s="24"/>
       <c r="O740" s="24"/>
       <c r="P740" s="24"/>
@@ -28551,8 +28594,8 @@
       <c r="T740" s="25"/>
       <c r="U740" s="25"/>
       <c r="V740" s="26"/>
-      <c r="W740" s="90" t="s">
-        <v>507</v>
+      <c r="W740" s="89" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="741" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28568,7 +28611,7 @@
       <c r="J741" s="31"/>
       <c r="K741" s="31"/>
       <c r="L741" s="31"/>
-      <c r="M741" s="91"/>
+      <c r="M741" s="90"/>
       <c r="N741" s="32"/>
       <c r="O741" s="32"/>
       <c r="P741" s="32"/>
@@ -28582,10 +28625,10 @@
     </row>
     <row r="742" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A742" s="10" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B742" s="11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C742" s="12">
         <v>0</v>
@@ -28645,10 +28688,10 @@
         <v>100</v>
       </c>
       <c r="V742" s="17" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="W742" s="18" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="743" spans="1:23" ht="132" thickBot="1" x14ac:dyDescent="0.3">
@@ -28675,7 +28718,7 @@
       <c r="U743" s="25"/>
       <c r="V743" s="26"/>
       <c r="W743" s="18" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="744" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -28756,7 +28799,7 @@
     <row r="747" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A747" s="19"/>
       <c r="B747" s="11" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C747" s="12">
         <v>0</v>
@@ -28780,13 +28823,13 @@
         <v>20</v>
       </c>
       <c r="J747" s="14" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="K747" s="14">
         <v>17</v>
       </c>
       <c r="L747" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="M747" s="14">
         <v>14</v>
@@ -28816,10 +28859,10 @@
         <v>60</v>
       </c>
       <c r="V747" s="17" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="W747" s="18" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="748" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -28925,7 +28968,7 @@
     <row r="752" spans="1:23" ht="244.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A752" s="19"/>
       <c r="B752" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C752" s="12">
         <v>0</v>
@@ -28985,10 +29028,10 @@
         <v>70</v>
       </c>
       <c r="V752" s="17" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="W752" s="18" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="753" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -29015,7 +29058,7 @@
       <c r="U753" s="25"/>
       <c r="V753" s="26"/>
       <c r="W753" s="18" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="754" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -29096,7 +29139,7 @@
     <row r="757" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A757" s="19"/>
       <c r="B757" s="11" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C757" s="12">
         <v>0</v>
@@ -29156,10 +29199,10 @@
         <v>60</v>
       </c>
       <c r="V757" s="17" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="W757" s="18" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="758" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -29265,7 +29308,7 @@
     <row r="762" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A762" s="19"/>
       <c r="B762" s="11" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C762" s="12">
         <v>0</v>
@@ -29304,13 +29347,13 @@
         <v>20</v>
       </c>
       <c r="O762" s="15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P762" s="15">
         <v>17</v>
       </c>
       <c r="Q762" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="R762" s="15">
         <v>14</v>
@@ -29430,7 +29473,7 @@
     <row r="767" spans="1:23" ht="294" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A767" s="19"/>
       <c r="B767" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C767" s="12">
         <v>0</v>
@@ -29490,10 +29533,10 @@
         <v>90</v>
       </c>
       <c r="V767" s="17" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="W767" s="18" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="768" spans="1:23" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -29520,7 +29563,7 @@
       <c r="U768" s="25"/>
       <c r="V768" s="26"/>
       <c r="W768" s="18" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="769" spans="1:23" ht="188.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -29547,7 +29590,7 @@
       <c r="U769" s="25"/>
       <c r="V769" s="26"/>
       <c r="W769" s="18" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="770" spans="1:23" ht="207" thickBot="1" x14ac:dyDescent="0.3">
@@ -29574,7 +29617,7 @@
       <c r="U770" s="25"/>
       <c r="V770" s="26"/>
       <c r="W770" s="18" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="771" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -29605,7 +29648,7 @@
     <row r="772" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A772" s="19"/>
       <c r="B772" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C772" s="12">
         <v>0</v>
@@ -29768,9 +29811,9 @@
       <c r="W776" s="35"/>
     </row>
     <row r="777" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A777" s="93"/>
+      <c r="A777" s="91"/>
       <c r="B777" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C777" s="12">
         <v>0</v>
@@ -29830,10 +29873,10 @@
         <v>80</v>
       </c>
       <c r="V777" s="17"/>
-      <c r="W777" s="93"/>
+      <c r="W777" s="91"/>
     </row>
     <row r="778" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A778" s="93"/>
+      <c r="A778" s="91"/>
       <c r="B778" s="20"/>
       <c r="C778" s="21"/>
       <c r="D778" s="22"/>
@@ -29855,10 +29898,10 @@
       <c r="T778" s="25"/>
       <c r="U778" s="25"/>
       <c r="V778" s="26"/>
-      <c r="W778" s="93"/>
+      <c r="W778" s="91"/>
     </row>
     <row r="779" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A779" s="93"/>
+      <c r="A779" s="91"/>
       <c r="B779" s="20"/>
       <c r="C779" s="21"/>
       <c r="D779" s="22"/>
@@ -29880,10 +29923,10 @@
       <c r="T779" s="25"/>
       <c r="U779" s="25"/>
       <c r="V779" s="26"/>
-      <c r="W779" s="93"/>
+      <c r="W779" s="91"/>
     </row>
     <row r="780" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A780" s="93"/>
+      <c r="A780" s="91"/>
       <c r="B780" s="20"/>
       <c r="C780" s="21"/>
       <c r="D780" s="22"/>
@@ -29905,10 +29948,10 @@
       <c r="T780" s="25"/>
       <c r="U780" s="25"/>
       <c r="V780" s="26"/>
-      <c r="W780" s="93"/>
+      <c r="W780" s="91"/>
     </row>
     <row r="781" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A781" s="95"/>
+      <c r="A781" s="93"/>
       <c r="B781" s="28"/>
       <c r="C781" s="29"/>
       <c r="D781" s="30"/>
@@ -29930,12 +29973,12 @@
       <c r="T781" s="51"/>
       <c r="U781" s="51"/>
       <c r="V781" s="34"/>
-      <c r="W781" s="93"/>
+      <c r="W781" s="91"/>
     </row>
     <row r="782" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A782" s="19"/>
       <c r="B782" s="11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C782" s="12">
         <v>0</v>
@@ -29995,7 +30038,7 @@
         <v>80</v>
       </c>
       <c r="V782" s="17"/>
-      <c r="W782" s="93"/>
+      <c r="W782" s="91"/>
     </row>
     <row r="783" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A783" s="19"/>
@@ -30020,7 +30063,7 @@
       <c r="T783" s="25"/>
       <c r="U783" s="25"/>
       <c r="V783" s="26"/>
-      <c r="W783" s="93"/>
+      <c r="W783" s="91"/>
     </row>
     <row r="784" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A784" s="19"/>
@@ -30045,7 +30088,7 @@
       <c r="T784" s="25"/>
       <c r="U784" s="25"/>
       <c r="V784" s="26"/>
-      <c r="W784" s="93"/>
+      <c r="W784" s="91"/>
     </row>
     <row r="785" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A785" s="19"/>
@@ -30070,7 +30113,7 @@
       <c r="T785" s="25"/>
       <c r="U785" s="25"/>
       <c r="V785" s="26"/>
-      <c r="W785" s="93"/>
+      <c r="W785" s="91"/>
     </row>
     <row r="786" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A786" s="27"/>
@@ -30095,12 +30138,12 @@
       <c r="T786" s="51"/>
       <c r="U786" s="51"/>
       <c r="V786" s="34"/>
-      <c r="W786" s="93"/>
+      <c r="W786" s="91"/>
     </row>
     <row r="787" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A787" s="19"/>
       <c r="B787" s="11" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C787" s="12">
         <v>0</v>
@@ -30160,7 +30203,7 @@
         <v>110</v>
       </c>
       <c r="V787" s="17"/>
-      <c r="W787" s="93"/>
+      <c r="W787" s="91"/>
     </row>
     <row r="788" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A788" s="19"/>
@@ -30185,7 +30228,7 @@
       <c r="T788" s="25"/>
       <c r="U788" s="25"/>
       <c r="V788" s="26"/>
-      <c r="W788" s="93"/>
+      <c r="W788" s="91"/>
     </row>
     <row r="789" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A789" s="19"/>
@@ -30210,7 +30253,7 @@
       <c r="T789" s="25"/>
       <c r="U789" s="25"/>
       <c r="V789" s="26"/>
-      <c r="W789" s="93"/>
+      <c r="W789" s="91"/>
     </row>
     <row r="790" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A790" s="19"/>
@@ -30235,7 +30278,7 @@
       <c r="T790" s="25"/>
       <c r="U790" s="25"/>
       <c r="V790" s="26"/>
-      <c r="W790" s="93"/>
+      <c r="W790" s="91"/>
     </row>
     <row r="791" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A791" s="27"/>
@@ -30260,74 +30303,74 @@
       <c r="T791" s="51"/>
       <c r="U791" s="51"/>
       <c r="V791" s="34"/>
-      <c r="W791" s="93"/>
+      <c r="W791" s="91"/>
     </row>
     <row r="792" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A792" s="19"/>
       <c r="B792" s="11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C792" s="12">
         <v>0</v>
       </c>
       <c r="D792" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E792" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F792" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G792" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H792" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I792" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J792" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K792" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L792" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="M792" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="N792" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="O792" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="P792" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="Q792" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="R792" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="S792" s="16" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="T792" s="16" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="U792" s="16" t="s">
-        <v>543</v>
-      </c>
-      <c r="V792" s="94" t="s">
-        <v>543</v>
-      </c>
-      <c r="W792" s="93"/>
+        <v>541</v>
+      </c>
+      <c r="V792" s="92" t="s">
+        <v>541</v>
+      </c>
+      <c r="W792" s="91"/>
     </row>
     <row r="793" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A793" s="19"/>
@@ -30351,8 +30394,8 @@
       <c r="S793" s="25"/>
       <c r="T793" s="25"/>
       <c r="U793" s="25"/>
-      <c r="V793" s="94"/>
-      <c r="W793" s="93"/>
+      <c r="V793" s="92"/>
+      <c r="W793" s="91"/>
     </row>
     <row r="794" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A794" s="19"/>
@@ -30376,8 +30419,8 @@
       <c r="S794" s="25"/>
       <c r="T794" s="25"/>
       <c r="U794" s="25"/>
-      <c r="V794" s="94"/>
-      <c r="W794" s="93"/>
+      <c r="V794" s="92"/>
+      <c r="W794" s="91"/>
     </row>
     <row r="795" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A795" s="19"/>
@@ -30401,8 +30444,8 @@
       <c r="S795" s="25"/>
       <c r="T795" s="25"/>
       <c r="U795" s="25"/>
-      <c r="V795" s="94"/>
-      <c r="W795" s="93"/>
+      <c r="V795" s="92"/>
+      <c r="W795" s="91"/>
     </row>
     <row r="796" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A796" s="27"/>
@@ -30427,7 +30470,7 @@
       <c r="T796" s="51"/>
       <c r="U796" s="51"/>
       <c r="V796" s="79"/>
-      <c r="W796" s="95"/>
+      <c r="W796" s="93"/>
     </row>
     <row r="797" spans="1:23" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A797" s="19"/>
@@ -30492,7 +30535,7 @@
         <v>120</v>
       </c>
       <c r="V797" s="17" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="W797" s="18" t="s">
         <v>206</v>
@@ -30601,7 +30644,7 @@
       <c r="W801" s="35"/>
     </row>
     <row r="802" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A802" s="93"/>
+      <c r="A802" s="91"/>
       <c r="B802" s="20"/>
       <c r="C802" s="21"/>
       <c r="D802" s="22"/>
@@ -30623,10 +30666,10 @@
       <c r="T802" s="25"/>
       <c r="U802" s="25"/>
       <c r="V802" s="26"/>
-      <c r="W802" s="93"/>
+      <c r="W802" s="91"/>
     </row>
     <row r="803" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A803" s="93"/>
+      <c r="A803" s="91"/>
       <c r="B803" s="20"/>
       <c r="C803" s="21"/>
       <c r="D803" s="22"/>
@@ -30648,10 +30691,10 @@
       <c r="T803" s="25"/>
       <c r="U803" s="25"/>
       <c r="V803" s="26"/>
-      <c r="W803" s="93"/>
+      <c r="W803" s="91"/>
     </row>
     <row r="804" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A804" s="93"/>
+      <c r="A804" s="91"/>
       <c r="B804" s="20"/>
       <c r="C804" s="21"/>
       <c r="D804" s="22"/>
@@ -30673,10 +30716,10 @@
       <c r="T804" s="25"/>
       <c r="U804" s="25"/>
       <c r="V804" s="26"/>
-      <c r="W804" s="93"/>
+      <c r="W804" s="91"/>
     </row>
     <row r="805" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A805" s="93"/>
+      <c r="A805" s="91"/>
       <c r="B805" s="20"/>
       <c r="C805" s="21"/>
       <c r="D805" s="22"/>
@@ -30698,10 +30741,10 @@
       <c r="T805" s="25"/>
       <c r="U805" s="25"/>
       <c r="V805" s="26"/>
-      <c r="W805" s="93"/>
+      <c r="W805" s="91"/>
     </row>
     <row r="806" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A806" s="93"/>
+      <c r="A806" s="91"/>
       <c r="B806" s="20"/>
       <c r="C806" s="21"/>
       <c r="D806" s="22"/>
@@ -30723,10 +30766,10 @@
       <c r="T806" s="25"/>
       <c r="U806" s="25"/>
       <c r="V806" s="26"/>
-      <c r="W806" s="93"/>
+      <c r="W806" s="91"/>
     </row>
     <row r="807" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A807" s="93"/>
+      <c r="A807" s="91"/>
       <c r="B807" s="20"/>
       <c r="C807" s="21"/>
       <c r="D807" s="22"/>
@@ -30748,10 +30791,10 @@
       <c r="T807" s="25"/>
       <c r="U807" s="25"/>
       <c r="V807" s="26"/>
-      <c r="W807" s="93"/>
+      <c r="W807" s="91"/>
     </row>
     <row r="808" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A808" s="93"/>
+      <c r="A808" s="91"/>
       <c r="B808" s="20"/>
       <c r="C808" s="21"/>
       <c r="D808" s="22"/>
@@ -30773,10 +30816,10 @@
       <c r="T808" s="25"/>
       <c r="U808" s="25"/>
       <c r="V808" s="26"/>
-      <c r="W808" s="93"/>
+      <c r="W808" s="91"/>
     </row>
     <row r="809" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A809" s="93"/>
+      <c r="A809" s="91"/>
       <c r="B809" s="20"/>
       <c r="C809" s="21"/>
       <c r="D809" s="22"/>
@@ -30798,10 +30841,10 @@
       <c r="T809" s="25"/>
       <c r="U809" s="25"/>
       <c r="V809" s="26"/>
-      <c r="W809" s="93"/>
+      <c r="W809" s="91"/>
     </row>
     <row r="810" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A810" s="93"/>
+      <c r="A810" s="91"/>
       <c r="B810" s="20"/>
       <c r="C810" s="21"/>
       <c r="D810" s="22"/>
@@ -30823,10 +30866,10 @@
       <c r="T810" s="25"/>
       <c r="U810" s="25"/>
       <c r="V810" s="26"/>
-      <c r="W810" s="93"/>
+      <c r="W810" s="91"/>
     </row>
     <row r="811" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A811" s="93"/>
+      <c r="A811" s="91"/>
       <c r="B811" s="20"/>
       <c r="C811" s="21"/>
       <c r="D811" s="22"/>
@@ -30848,10 +30891,10 @@
       <c r="T811" s="25"/>
       <c r="U811" s="25"/>
       <c r="V811" s="26"/>
-      <c r="W811" s="93"/>
+      <c r="W811" s="91"/>
     </row>
     <row r="812" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A812" s="93"/>
+      <c r="A812" s="91"/>
       <c r="B812" s="20"/>
       <c r="C812" s="21"/>
       <c r="D812" s="22"/>
@@ -30873,10 +30916,10 @@
       <c r="T812" s="25"/>
       <c r="U812" s="25"/>
       <c r="V812" s="26"/>
-      <c r="W812" s="93"/>
+      <c r="W812" s="91"/>
     </row>
     <row r="813" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A813" s="93"/>
+      <c r="A813" s="91"/>
       <c r="B813" s="20"/>
       <c r="C813" s="21"/>
       <c r="D813" s="22"/>
@@ -30898,10 +30941,10 @@
       <c r="T813" s="25"/>
       <c r="U813" s="25"/>
       <c r="V813" s="26"/>
-      <c r="W813" s="93"/>
+      <c r="W813" s="91"/>
     </row>
     <row r="814" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A814" s="93"/>
+      <c r="A814" s="91"/>
       <c r="B814" s="20"/>
       <c r="C814" s="21"/>
       <c r="D814" s="22"/>
@@ -30923,10 +30966,10 @@
       <c r="T814" s="25"/>
       <c r="U814" s="25"/>
       <c r="V814" s="26"/>
-      <c r="W814" s="93"/>
+      <c r="W814" s="91"/>
     </row>
     <row r="815" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A815" s="93"/>
+      <c r="A815" s="91"/>
       <c r="B815" s="20"/>
       <c r="C815" s="21"/>
       <c r="D815" s="22"/>
@@ -30948,10 +30991,10 @@
       <c r="T815" s="25"/>
       <c r="U815" s="25"/>
       <c r="V815" s="26"/>
-      <c r="W815" s="93"/>
+      <c r="W815" s="91"/>
     </row>
     <row r="816" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A816" s="93"/>
+      <c r="A816" s="91"/>
       <c r="B816" s="20"/>
       <c r="C816" s="21"/>
       <c r="D816" s="22"/>
@@ -30973,10 +31016,10 @@
       <c r="T816" s="25"/>
       <c r="U816" s="25"/>
       <c r="V816" s="26"/>
-      <c r="W816" s="93"/>
+      <c r="W816" s="91"/>
     </row>
     <row r="817" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A817" s="93"/>
+      <c r="A817" s="91"/>
       <c r="B817" s="20"/>
       <c r="C817" s="21"/>
       <c r="D817" s="22"/>
@@ -30998,10 +31041,10 @@
       <c r="T817" s="25"/>
       <c r="U817" s="25"/>
       <c r="V817" s="26"/>
-      <c r="W817" s="93"/>
+      <c r="W817" s="91"/>
     </row>
     <row r="818" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A818" s="93"/>
+      <c r="A818" s="91"/>
       <c r="B818" s="20"/>
       <c r="C818" s="21"/>
       <c r="D818" s="22"/>
@@ -31023,10 +31066,10 @@
       <c r="T818" s="25"/>
       <c r="U818" s="25"/>
       <c r="V818" s="26"/>
-      <c r="W818" s="93"/>
+      <c r="W818" s="91"/>
     </row>
     <row r="819" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A819" s="93"/>
+      <c r="A819" s="91"/>
       <c r="B819" s="20"/>
       <c r="C819" s="21"/>
       <c r="D819" s="22"/>
@@ -31048,10 +31091,10 @@
       <c r="T819" s="25"/>
       <c r="U819" s="25"/>
       <c r="V819" s="26"/>
-      <c r="W819" s="93"/>
+      <c r="W819" s="91"/>
     </row>
     <row r="820" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A820" s="93"/>
+      <c r="A820" s="91"/>
       <c r="B820" s="20"/>
       <c r="C820" s="21"/>
       <c r="D820" s="22"/>
@@ -31073,10 +31116,10 @@
       <c r="T820" s="25"/>
       <c r="U820" s="25"/>
       <c r="V820" s="26"/>
-      <c r="W820" s="93"/>
+      <c r="W820" s="91"/>
     </row>
     <row r="821" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A821" s="93"/>
+      <c r="A821" s="91"/>
       <c r="B821" s="20"/>
       <c r="C821" s="21"/>
       <c r="D821" s="22"/>
@@ -31098,10 +31141,10 @@
       <c r="T821" s="25"/>
       <c r="U821" s="25"/>
       <c r="V821" s="26"/>
-      <c r="W821" s="93"/>
+      <c r="W821" s="91"/>
     </row>
     <row r="822" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A822" s="93"/>
+      <c r="A822" s="91"/>
       <c r="B822" s="20"/>
       <c r="C822" s="21"/>
       <c r="D822" s="22"/>
@@ -31123,10 +31166,10 @@
       <c r="T822" s="25"/>
       <c r="U822" s="25"/>
       <c r="V822" s="26"/>
-      <c r="W822" s="93"/>
+      <c r="W822" s="91"/>
     </row>
     <row r="823" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A823" s="93"/>
+      <c r="A823" s="91"/>
       <c r="B823" s="20"/>
       <c r="C823" s="21"/>
       <c r="D823" s="22"/>
@@ -31148,10 +31191,10 @@
       <c r="T823" s="25"/>
       <c r="U823" s="25"/>
       <c r="V823" s="26"/>
-      <c r="W823" s="93"/>
+      <c r="W823" s="91"/>
     </row>
     <row r="824" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A824" s="93"/>
+      <c r="A824" s="91"/>
       <c r="B824" s="20"/>
       <c r="C824" s="21"/>
       <c r="D824" s="22"/>
@@ -31173,10 +31216,10 @@
       <c r="T824" s="25"/>
       <c r="U824" s="25"/>
       <c r="V824" s="26"/>
-      <c r="W824" s="93"/>
+      <c r="W824" s="91"/>
     </row>
     <row r="825" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A825" s="93"/>
+      <c r="A825" s="91"/>
       <c r="B825" s="20"/>
       <c r="C825" s="21"/>
       <c r="D825" s="22"/>
@@ -31198,10 +31241,10 @@
       <c r="T825" s="25"/>
       <c r="U825" s="25"/>
       <c r="V825" s="26"/>
-      <c r="W825" s="93"/>
+      <c r="W825" s="91"/>
     </row>
     <row r="826" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A826" s="93"/>
+      <c r="A826" s="91"/>
       <c r="B826" s="20"/>
       <c r="C826" s="21"/>
       <c r="D826" s="22"/>
@@ -31223,10 +31266,10 @@
       <c r="T826" s="25"/>
       <c r="U826" s="25"/>
       <c r="V826" s="26"/>
-      <c r="W826" s="93"/>
+      <c r="W826" s="91"/>
     </row>
     <row r="827" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A827" s="93"/>
+      <c r="A827" s="91"/>
       <c r="B827" s="20"/>
       <c r="C827" s="21"/>
       <c r="D827" s="22"/>
@@ -31248,10 +31291,10 @@
       <c r="T827" s="25"/>
       <c r="U827" s="25"/>
       <c r="V827" s="26"/>
-      <c r="W827" s="93"/>
+      <c r="W827" s="91"/>
     </row>
     <row r="828" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A828" s="93"/>
+      <c r="A828" s="91"/>
       <c r="B828" s="20"/>
       <c r="C828" s="21"/>
       <c r="D828" s="22"/>
@@ -31273,10 +31316,10 @@
       <c r="T828" s="25"/>
       <c r="U828" s="25"/>
       <c r="V828" s="26"/>
-      <c r="W828" s="93"/>
+      <c r="W828" s="91"/>
     </row>
     <row r="829" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A829" s="93"/>
+      <c r="A829" s="91"/>
       <c r="B829" s="20"/>
       <c r="C829" s="21"/>
       <c r="D829" s="22"/>
@@ -31298,10 +31341,10 @@
       <c r="T829" s="25"/>
       <c r="U829" s="25"/>
       <c r="V829" s="26"/>
-      <c r="W829" s="93"/>
+      <c r="W829" s="91"/>
     </row>
     <row r="830" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A830" s="93"/>
+      <c r="A830" s="91"/>
       <c r="B830" s="20"/>
       <c r="C830" s="21"/>
       <c r="D830" s="22"/>
@@ -31323,10 +31366,10 @@
       <c r="T830" s="25"/>
       <c r="U830" s="25"/>
       <c r="V830" s="26"/>
-      <c r="W830" s="93"/>
+      <c r="W830" s="91"/>
     </row>
     <row r="831" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A831" s="93"/>
+      <c r="A831" s="91"/>
       <c r="B831" s="20"/>
       <c r="C831" s="21"/>
       <c r="D831" s="22"/>
@@ -31348,10 +31391,10 @@
       <c r="T831" s="25"/>
       <c r="U831" s="25"/>
       <c r="V831" s="26"/>
-      <c r="W831" s="93"/>
+      <c r="W831" s="91"/>
     </row>
     <row r="832" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A832" s="93"/>
+      <c r="A832" s="91"/>
       <c r="B832" s="20"/>
       <c r="C832" s="21"/>
       <c r="D832" s="22"/>
@@ -31373,10 +31416,10 @@
       <c r="T832" s="25"/>
       <c r="U832" s="25"/>
       <c r="V832" s="26"/>
-      <c r="W832" s="93"/>
+      <c r="W832" s="91"/>
     </row>
     <row r="833" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A833" s="93"/>
+      <c r="A833" s="91"/>
       <c r="B833" s="20"/>
       <c r="C833" s="21"/>
       <c r="D833" s="22"/>
@@ -31398,10 +31441,10 @@
       <c r="T833" s="25"/>
       <c r="U833" s="25"/>
       <c r="V833" s="26"/>
-      <c r="W833" s="93"/>
+      <c r="W833" s="91"/>
     </row>
     <row r="834" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A834" s="93"/>
+      <c r="A834" s="91"/>
       <c r="B834" s="20"/>
       <c r="C834" s="21"/>
       <c r="D834" s="22"/>
@@ -31423,10 +31466,10 @@
       <c r="T834" s="25"/>
       <c r="U834" s="25"/>
       <c r="V834" s="26"/>
-      <c r="W834" s="93"/>
+      <c r="W834" s="91"/>
     </row>
     <row r="835" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A835" s="93"/>
+      <c r="A835" s="91"/>
       <c r="B835" s="20"/>
       <c r="C835" s="21"/>
       <c r="D835" s="22"/>
@@ -31448,10 +31491,10 @@
       <c r="T835" s="25"/>
       <c r="U835" s="25"/>
       <c r="V835" s="26"/>
-      <c r="W835" s="93"/>
+      <c r="W835" s="91"/>
     </row>
     <row r="836" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A836" s="93"/>
+      <c r="A836" s="91"/>
       <c r="B836" s="20"/>
       <c r="C836" s="21"/>
       <c r="D836" s="22"/>
@@ -31473,10 +31516,10 @@
       <c r="T836" s="25"/>
       <c r="U836" s="25"/>
       <c r="V836" s="26"/>
-      <c r="W836" s="93"/>
+      <c r="W836" s="91"/>
     </row>
     <row r="837" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A837" s="93"/>
+      <c r="A837" s="91"/>
       <c r="B837" s="20"/>
       <c r="C837" s="21"/>
       <c r="D837" s="22"/>
@@ -31498,10 +31541,10 @@
       <c r="T837" s="25"/>
       <c r="U837" s="25"/>
       <c r="V837" s="26"/>
-      <c r="W837" s="93"/>
+      <c r="W837" s="91"/>
     </row>
     <row r="838" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A838" s="93"/>
+      <c r="A838" s="91"/>
       <c r="B838" s="20"/>
       <c r="C838" s="21"/>
       <c r="D838" s="22"/>
@@ -31523,10 +31566,10 @@
       <c r="T838" s="25"/>
       <c r="U838" s="25"/>
       <c r="V838" s="26"/>
-      <c r="W838" s="93"/>
+      <c r="W838" s="91"/>
     </row>
     <row r="839" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A839" s="93"/>
+      <c r="A839" s="91"/>
       <c r="B839" s="20"/>
       <c r="C839" s="21"/>
       <c r="D839" s="22"/>
@@ -31548,10 +31591,10 @@
       <c r="T839" s="25"/>
       <c r="U839" s="25"/>
       <c r="V839" s="26"/>
-      <c r="W839" s="93"/>
+      <c r="W839" s="91"/>
     </row>
     <row r="840" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A840" s="93"/>
+      <c r="A840" s="91"/>
       <c r="B840" s="20"/>
       <c r="C840" s="21"/>
       <c r="D840" s="22"/>
@@ -31573,10 +31616,10 @@
       <c r="T840" s="25"/>
       <c r="U840" s="25"/>
       <c r="V840" s="26"/>
-      <c r="W840" s="93"/>
+      <c r="W840" s="91"/>
     </row>
     <row r="841" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A841" s="93"/>
+      <c r="A841" s="91"/>
       <c r="B841" s="20"/>
       <c r="C841" s="21"/>
       <c r="D841" s="22"/>
@@ -31598,10 +31641,10 @@
       <c r="T841" s="25"/>
       <c r="U841" s="25"/>
       <c r="V841" s="26"/>
-      <c r="W841" s="93"/>
+      <c r="W841" s="91"/>
     </row>
     <row r="842" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A842" s="93"/>
+      <c r="A842" s="91"/>
       <c r="B842" s="20"/>
       <c r="C842" s="21"/>
       <c r="D842" s="22"/>
@@ -31623,10 +31666,10 @@
       <c r="T842" s="25"/>
       <c r="U842" s="25"/>
       <c r="V842" s="26"/>
-      <c r="W842" s="93"/>
+      <c r="W842" s="91"/>
     </row>
     <row r="843" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A843" s="93"/>
+      <c r="A843" s="91"/>
       <c r="B843" s="20"/>
       <c r="C843" s="21"/>
       <c r="D843" s="22"/>
@@ -31648,10 +31691,10 @@
       <c r="T843" s="25"/>
       <c r="U843" s="25"/>
       <c r="V843" s="26"/>
-      <c r="W843" s="93"/>
+      <c r="W843" s="91"/>
     </row>
     <row r="844" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A844" s="93"/>
+      <c r="A844" s="91"/>
       <c r="B844" s="20"/>
       <c r="C844" s="21"/>
       <c r="D844" s="22"/>
@@ -31673,10 +31716,10 @@
       <c r="T844" s="25"/>
       <c r="U844" s="25"/>
       <c r="V844" s="26"/>
-      <c r="W844" s="93"/>
+      <c r="W844" s="91"/>
     </row>
     <row r="845" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A845" s="93"/>
+      <c r="A845" s="91"/>
       <c r="B845" s="20"/>
       <c r="C845" s="21"/>
       <c r="D845" s="22"/>
@@ -31698,10 +31741,10 @@
       <c r="T845" s="25"/>
       <c r="U845" s="25"/>
       <c r="V845" s="26"/>
-      <c r="W845" s="93"/>
+      <c r="W845" s="91"/>
     </row>
     <row r="846" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A846" s="93"/>
+      <c r="A846" s="91"/>
       <c r="B846" s="20"/>
       <c r="C846" s="21"/>
       <c r="D846" s="22"/>
@@ -31723,10 +31766,10 @@
       <c r="T846" s="25"/>
       <c r="U846" s="25"/>
       <c r="V846" s="26"/>
-      <c r="W846" s="93"/>
+      <c r="W846" s="91"/>
     </row>
     <row r="847" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A847" s="93"/>
+      <c r="A847" s="91"/>
       <c r="B847" s="20"/>
       <c r="C847" s="21"/>
       <c r="D847" s="22"/>
@@ -31748,10 +31791,10 @@
       <c r="T847" s="25"/>
       <c r="U847" s="25"/>
       <c r="V847" s="26"/>
-      <c r="W847" s="93"/>
+      <c r="W847" s="91"/>
     </row>
     <row r="848" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A848" s="93"/>
+      <c r="A848" s="91"/>
       <c r="B848" s="20"/>
       <c r="C848" s="21"/>
       <c r="D848" s="22"/>
@@ -31773,10 +31816,10 @@
       <c r="T848" s="25"/>
       <c r="U848" s="25"/>
       <c r="V848" s="26"/>
-      <c r="W848" s="93"/>
+      <c r="W848" s="91"/>
     </row>
     <row r="849" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A849" s="93"/>
+      <c r="A849" s="91"/>
       <c r="B849" s="20"/>
       <c r="C849" s="21"/>
       <c r="D849" s="22"/>
@@ -31798,10 +31841,10 @@
       <c r="T849" s="25"/>
       <c r="U849" s="25"/>
       <c r="V849" s="26"/>
-      <c r="W849" s="93"/>
+      <c r="W849" s="91"/>
     </row>
     <row r="850" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A850" s="93"/>
+      <c r="A850" s="91"/>
       <c r="B850" s="20"/>
       <c r="C850" s="21"/>
       <c r="D850" s="22"/>
@@ -31823,10 +31866,10 @@
       <c r="T850" s="25"/>
       <c r="U850" s="25"/>
       <c r="V850" s="26"/>
-      <c r="W850" s="93"/>
+      <c r="W850" s="91"/>
     </row>
     <row r="851" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A851" s="93"/>
+      <c r="A851" s="91"/>
       <c r="B851" s="20"/>
       <c r="C851" s="21"/>
       <c r="D851" s="22"/>
@@ -31848,10 +31891,10 @@
       <c r="T851" s="25"/>
       <c r="U851" s="25"/>
       <c r="V851" s="26"/>
-      <c r="W851" s="93"/>
+      <c r="W851" s="91"/>
     </row>
     <row r="852" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A852" s="93"/>
+      <c r="A852" s="91"/>
       <c r="B852" s="20"/>
       <c r="C852" s="21"/>
       <c r="D852" s="22"/>
@@ -31873,10 +31916,10 @@
       <c r="T852" s="25"/>
       <c r="U852" s="25"/>
       <c r="V852" s="26"/>
-      <c r="W852" s="93"/>
+      <c r="W852" s="91"/>
     </row>
     <row r="853" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A853" s="93"/>
+      <c r="A853" s="91"/>
       <c r="B853" s="20"/>
       <c r="C853" s="21"/>
       <c r="D853" s="22"/>
@@ -31898,10 +31941,10 @@
       <c r="T853" s="25"/>
       <c r="U853" s="25"/>
       <c r="V853" s="26"/>
-      <c r="W853" s="93"/>
+      <c r="W853" s="91"/>
     </row>
     <row r="854" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A854" s="93"/>
+      <c r="A854" s="91"/>
       <c r="B854" s="20"/>
       <c r="C854" s="21"/>
       <c r="D854" s="22"/>
@@ -31923,10 +31966,10 @@
       <c r="T854" s="25"/>
       <c r="U854" s="25"/>
       <c r="V854" s="26"/>
-      <c r="W854" s="93"/>
+      <c r="W854" s="91"/>
     </row>
     <row r="855" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A855" s="93"/>
+      <c r="A855" s="91"/>
       <c r="B855" s="20"/>
       <c r="C855" s="21"/>
       <c r="D855" s="22"/>
@@ -31948,10 +31991,10 @@
       <c r="T855" s="25"/>
       <c r="U855" s="25"/>
       <c r="V855" s="26"/>
-      <c r="W855" s="93"/>
+      <c r="W855" s="91"/>
     </row>
     <row r="856" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A856" s="93"/>
+      <c r="A856" s="91"/>
       <c r="B856" s="20"/>
       <c r="C856" s="21"/>
       <c r="D856" s="22"/>
@@ -31973,10 +32016,10 @@
       <c r="T856" s="25"/>
       <c r="U856" s="25"/>
       <c r="V856" s="26"/>
-      <c r="W856" s="93"/>
+      <c r="W856" s="91"/>
     </row>
     <row r="857" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A857" s="93"/>
+      <c r="A857" s="91"/>
       <c r="B857" s="20"/>
       <c r="C857" s="21"/>
       <c r="D857" s="22"/>
@@ -31998,10 +32041,10 @@
       <c r="T857" s="25"/>
       <c r="U857" s="25"/>
       <c r="V857" s="26"/>
-      <c r="W857" s="93"/>
+      <c r="W857" s="91"/>
     </row>
     <row r="858" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A858" s="93"/>
+      <c r="A858" s="91"/>
       <c r="B858" s="20"/>
       <c r="C858" s="21"/>
       <c r="D858" s="22"/>
@@ -32023,10 +32066,10 @@
       <c r="T858" s="25"/>
       <c r="U858" s="25"/>
       <c r="V858" s="26"/>
-      <c r="W858" s="93"/>
+      <c r="W858" s="91"/>
     </row>
     <row r="859" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A859" s="93"/>
+      <c r="A859" s="91"/>
       <c r="B859" s="20"/>
       <c r="C859" s="21"/>
       <c r="D859" s="22"/>
@@ -32048,10 +32091,10 @@
       <c r="T859" s="25"/>
       <c r="U859" s="25"/>
       <c r="V859" s="26"/>
-      <c r="W859" s="93"/>
+      <c r="W859" s="91"/>
     </row>
     <row r="860" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A860" s="93"/>
+      <c r="A860" s="91"/>
       <c r="B860" s="20"/>
       <c r="C860" s="21"/>
       <c r="D860" s="22"/>
@@ -32073,10 +32116,10 @@
       <c r="T860" s="25"/>
       <c r="U860" s="25"/>
       <c r="V860" s="26"/>
-      <c r="W860" s="93"/>
+      <c r="W860" s="91"/>
     </row>
     <row r="861" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A861" s="93"/>
+      <c r="A861" s="91"/>
       <c r="B861" s="20"/>
       <c r="C861" s="21"/>
       <c r="D861" s="22"/>
@@ -32098,10 +32141,10 @@
       <c r="T861" s="25"/>
       <c r="U861" s="25"/>
       <c r="V861" s="26"/>
-      <c r="W861" s="93"/>
+      <c r="W861" s="91"/>
     </row>
     <row r="862" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A862" s="93"/>
+      <c r="A862" s="91"/>
       <c r="B862" s="20"/>
       <c r="C862" s="21"/>
       <c r="D862" s="22"/>
@@ -32123,10 +32166,10 @@
       <c r="T862" s="25"/>
       <c r="U862" s="25"/>
       <c r="V862" s="26"/>
-      <c r="W862" s="93"/>
+      <c r="W862" s="91"/>
     </row>
     <row r="863" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A863" s="93"/>
+      <c r="A863" s="91"/>
       <c r="B863" s="20"/>
       <c r="C863" s="21"/>
       <c r="D863" s="22"/>
@@ -32148,10 +32191,10 @@
       <c r="T863" s="25"/>
       <c r="U863" s="25"/>
       <c r="V863" s="26"/>
-      <c r="W863" s="93"/>
+      <c r="W863" s="91"/>
     </row>
     <row r="864" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A864" s="93"/>
+      <c r="A864" s="91"/>
       <c r="B864" s="20"/>
       <c r="C864" s="21"/>
       <c r="D864" s="22"/>
@@ -32173,10 +32216,10 @@
       <c r="T864" s="25"/>
       <c r="U864" s="25"/>
       <c r="V864" s="26"/>
-      <c r="W864" s="93"/>
+      <c r="W864" s="91"/>
     </row>
     <row r="865" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A865" s="93"/>
+      <c r="A865" s="91"/>
       <c r="B865" s="20"/>
       <c r="C865" s="21"/>
       <c r="D865" s="22"/>
@@ -32198,10 +32241,10 @@
       <c r="T865" s="25"/>
       <c r="U865" s="25"/>
       <c r="V865" s="26"/>
-      <c r="W865" s="93"/>
+      <c r="W865" s="91"/>
     </row>
     <row r="866" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A866" s="93"/>
+      <c r="A866" s="91"/>
       <c r="B866" s="20"/>
       <c r="C866" s="21"/>
       <c r="D866" s="22"/>
@@ -32223,10 +32266,10 @@
       <c r="T866" s="25"/>
       <c r="U866" s="25"/>
       <c r="V866" s="26"/>
-      <c r="W866" s="93"/>
+      <c r="W866" s="91"/>
     </row>
     <row r="867" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A867" s="93"/>
+      <c r="A867" s="91"/>
       <c r="B867" s="20"/>
       <c r="C867" s="21"/>
       <c r="D867" s="22"/>
@@ -32248,10 +32291,10 @@
       <c r="T867" s="25"/>
       <c r="U867" s="25"/>
       <c r="V867" s="26"/>
-      <c r="W867" s="93"/>
+      <c r="W867" s="91"/>
     </row>
     <row r="868" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A868" s="93"/>
+      <c r="A868" s="91"/>
       <c r="B868" s="20"/>
       <c r="C868" s="21"/>
       <c r="D868" s="22"/>
@@ -32273,10 +32316,10 @@
       <c r="T868" s="25"/>
       <c r="U868" s="25"/>
       <c r="V868" s="26"/>
-      <c r="W868" s="93"/>
+      <c r="W868" s="91"/>
     </row>
     <row r="869" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A869" s="93"/>
+      <c r="A869" s="91"/>
       <c r="B869" s="20"/>
       <c r="C869" s="21"/>
       <c r="D869" s="22"/>
@@ -32298,10 +32341,10 @@
       <c r="T869" s="25"/>
       <c r="U869" s="25"/>
       <c r="V869" s="26"/>
-      <c r="W869" s="93"/>
+      <c r="W869" s="91"/>
     </row>
     <row r="870" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A870" s="93"/>
+      <c r="A870" s="91"/>
       <c r="B870" s="20"/>
       <c r="C870" s="21"/>
       <c r="D870" s="22"/>
@@ -32323,10 +32366,10 @@
       <c r="T870" s="25"/>
       <c r="U870" s="25"/>
       <c r="V870" s="26"/>
-      <c r="W870" s="93"/>
+      <c r="W870" s="91"/>
     </row>
     <row r="871" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A871" s="93"/>
+      <c r="A871" s="91"/>
       <c r="B871" s="20"/>
       <c r="C871" s="21"/>
       <c r="D871" s="22"/>
@@ -32348,7 +32391,7 @@
       <c r="T871" s="25"/>
       <c r="U871" s="25"/>
       <c r="V871" s="26"/>
-      <c r="W871" s="93"/>
+      <c r="W871" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -32373,13 +32416,13 @@
     <mergeCell ref="I731:L731"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="W38" r:id="rId1" xr:uid="{FAB70775-25CD-4FCB-83F1-5010E806CB8E}"/>
-    <hyperlink ref="W212" r:id="rId2" xr:uid="{A884D4E3-BC72-4896-B2A0-6617D5F7A2CA}"/>
-    <hyperlink ref="W287" r:id="rId3" xr:uid="{FFD5939D-75F1-46D5-9823-E19AA09D95A2}"/>
-    <hyperlink ref="W292" r:id="rId4" xr:uid="{EBA51951-DB40-443E-99EF-07FC005E52EF}"/>
-    <hyperlink ref="W306" r:id="rId5" display="http://leagueoflegends.wikia.com/wiki/Kindred" xr:uid="{9C40BB66-2B41-4886-B603-06A647B8B433}"/>
-    <hyperlink ref="W441" r:id="rId6" xr:uid="{9E93812C-917D-4637-953F-F6EECAAA1C71}"/>
-    <hyperlink ref="W515" r:id="rId7" display="https://leagueoflegends.fandom.com/wiki/Samira" xr:uid="{C81FCCCE-9911-44CF-9BCB-ED8D43FD965E}"/>
+    <hyperlink ref="W38" r:id="rId1" xr:uid="{FF427DB6-9D6E-497B-947D-64AFA64905BA}"/>
+    <hyperlink ref="W212" r:id="rId2" xr:uid="{C8807BA6-60EC-49C4-9AF4-A7503A0B79BB}"/>
+    <hyperlink ref="W287" r:id="rId3" xr:uid="{7A7504A4-C9DB-4137-855F-0818F8A1B8D6}"/>
+    <hyperlink ref="W292" r:id="rId4" xr:uid="{75D8C68C-C2C6-48F5-93E9-89FEA61D10BA}"/>
+    <hyperlink ref="W306" r:id="rId5" display="http://leagueoflegends.wikia.com/wiki/Kindred" xr:uid="{8431D811-8094-4AA9-92D8-C04D162D4599}"/>
+    <hyperlink ref="W441" r:id="rId6" xr:uid="{FCCBC0B8-03D4-46BD-8143-62152D915AC1}"/>
+    <hyperlink ref="W515" r:id="rId7" display="https://leagueoflegends.fandom.com/wiki/Samira" xr:uid="{DA6C8C0E-3F63-482E-8A53-7A55319FD708}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>